<commit_message>
received parts on 04/20/2022.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="484">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -1553,13 +1553,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[$-C09]dd\-mmm\-yy"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1678,17 +1678,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1706,71 +1708,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1785,7 +1724,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1799,10 +1746,32 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1816,6 +1785,37 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1905,7 +1905,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1917,7 +1965,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1929,19 +2001,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1959,133 +2079,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2486,30 +2486,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2521,6 +2497,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2540,6 +2534,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2555,173 +2569,159 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="37" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="38" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2739,7 +2739,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2764,7 +2764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2790,7 +2790,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2889,14 +2889,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2920,7 +2920,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2935,7 +2935,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2959,61 +2959,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3112,16 +3112,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3148,16 +3148,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3427,10 +3427,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D92" activePane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
+      <pane ySplit="1170" topLeftCell="D40" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G124" sqref="G124"/>
+      <selection pane="bottomLeft" activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3549,7 +3549,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44671</v>
+        <v>44672</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -5280,21 +5280,27 @@
         <f t="shared" ref="K40:K71" si="9">$C$4*A40</f>
         <v>32</v>
       </c>
-      <c r="L40" s="110"/>
+      <c r="L40" s="110">
+        <v>32</v>
+      </c>
       <c r="M40" s="109">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N40" s="110"/>
+        <v>53.76</v>
+      </c>
+      <c r="N40" s="110">
+        <v>32</v>
+      </c>
       <c r="O40" s="110">
         <v>53.76</v>
       </c>
       <c r="P40" s="110"/>
       <c r="Q40" s="110">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R40" s="123"/>
+        <v>32</v>
+      </c>
+      <c r="R40" s="123" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" ht="12.75" customHeight="1" spans="1:18">
       <c r="A41" s="51">
@@ -8783,7 +8789,7 @@
         <v>1633.92</v>
       </c>
       <c r="N110" s="106">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O110" s="106">
         <v>1633.92</v>
@@ -8791,9 +8797,11 @@
       <c r="P110" s="106"/>
       <c r="Q110" s="106">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R110" s="121"/>
+        <v>32</v>
+      </c>
+      <c r="R110" s="121" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="111" ht="12.75" customHeight="1" spans="1:18">
       <c r="A111" s="51">
@@ -27213,7 +27221,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44671</v>
+        <v>44672</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
received some headers on 04/22/2022.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="484">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -1553,13 +1553,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="[$-C09]dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1678,26 +1678,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1708,8 +1722,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1724,17 +1739,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1746,10 +1761,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1769,15 +1792,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1785,37 +1816,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1905,19 +1905,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1929,139 +1923,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2079,13 +1947,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2486,30 +2486,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2534,11 +2510,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2550,21 +2532,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2583,148 +2550,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="27" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="37" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="27" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="33" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2739,7 +2739,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2764,7 +2764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2790,7 +2790,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2889,14 +2889,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2920,7 +2920,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2935,7 +2935,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2959,61 +2959,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3112,16 +3112,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3148,16 +3148,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3428,9 +3428,9 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D40" activePane="bottomLeft"/>
+      <pane ySplit="1170" topLeftCell="D32" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R40" sqref="R40"/>
+      <selection pane="bottomLeft" activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3549,7 +3549,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44672</v>
+        <v>44673</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -5129,7 +5129,7 @@
         <v>30</v>
       </c>
       <c r="N37" s="106">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O37" s="106">
         <v>9.6</v>
@@ -5137,9 +5137,11 @@
       <c r="P37" s="106"/>
       <c r="Q37" s="106">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R37" s="121"/>
+        <v>100</v>
+      </c>
+      <c r="R37" s="121" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="38" ht="14" customHeight="1" spans="1:18">
       <c r="A38" s="46">
@@ -27221,7 +27223,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44672</v>
+        <v>44673</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
received 6 LTC6090. Now, we received 128 LTC6090.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="483">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -836,9 +836,6 @@
     <t>3/16/2022</t>
   </si>
   <si>
-    <t>RAL Dig Lab(need 6 more)</t>
-  </si>
-  <si>
     <t>OPA2376AIDR</t>
   </si>
   <si>
@@ -1554,12 +1551,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1670,14 +1667,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1692,6 +1681,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1700,23 +1696,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1732,14 +1728,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1753,36 +1771,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1791,8 +1779,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1806,16 +1795,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1911,13 +1908,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1929,121 +1938,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2061,7 +1956,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2073,7 +1998,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2085,7 +2064,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2495,6 +2492,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2506,6 +2512,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2527,26 +2544,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2566,168 +2566,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="38" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="33" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2739,7 +2736,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2764,7 +2761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2790,7 +2787,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2962,58 +2959,58 @@
     <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3148,16 +3145,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3428,9 +3425,9 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D32" activePane="bottomLeft"/>
+      <pane ySplit="1170" topLeftCell="D71" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R37" sqref="R37"/>
+      <selection pane="bottomLeft" activeCell="R95" sqref="R95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3549,7 +3546,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44673</v>
+        <v>44678</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -7998,7 +7995,7 @@
         <v>1181.44</v>
       </c>
       <c r="N95" s="106">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="O95" s="106">
         <v>4725.76</v>
@@ -8008,10 +8005,10 @@
       </c>
       <c r="Q95" s="106">
         <f t="shared" si="15"/>
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="R95" s="121" t="s">
-        <v>259</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" ht="12.75" customHeight="1" spans="1:18">
@@ -8023,13 +8020,13 @@
       </c>
       <c r="C96" s="132"/>
       <c r="D96" s="132" t="s">
+        <v>259</v>
+      </c>
+      <c r="E96" s="132" t="s">
         <v>260</v>
       </c>
-      <c r="E96" s="132" t="s">
+      <c r="F96" s="132" t="s">
         <v>261</v>
-      </c>
-      <c r="F96" s="132" t="s">
-        <v>262</v>
       </c>
       <c r="G96" s="94" t="s">
         <v>26</v>
@@ -8064,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="R96" s="127" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97" ht="12.75" customHeight="1" spans="1:18">
@@ -8076,13 +8073,13 @@
       </c>
       <c r="C97" s="52"/>
       <c r="D97" s="53" t="s">
+        <v>263</v>
+      </c>
+      <c r="E97" s="53" t="s">
         <v>264</v>
       </c>
-      <c r="E97" s="53" t="s">
+      <c r="F97" s="53" t="s">
         <v>265</v>
-      </c>
-      <c r="F97" s="53" t="s">
-        <v>266</v>
       </c>
       <c r="G97" s="85" t="s">
         <v>26</v>
@@ -8133,13 +8130,13 @@
       </c>
       <c r="C98" s="134"/>
       <c r="D98" s="134" t="s">
+        <v>266</v>
+      </c>
+      <c r="E98" s="134" t="s">
         <v>267</v>
       </c>
-      <c r="E98" s="134" t="s">
+      <c r="F98" s="134" t="s">
         <v>268</v>
-      </c>
-      <c r="F98" s="134" t="s">
-        <v>269</v>
       </c>
       <c r="G98" s="149" t="s">
         <v>26</v>
@@ -8174,7 +8171,7 @@
         <v>2</v>
       </c>
       <c r="R98" s="165" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="99" ht="14" customHeight="1" spans="1:18">
@@ -8186,19 +8183,19 @@
       </c>
       <c r="C99" s="136"/>
       <c r="D99" s="137" t="s">
+        <v>270</v>
+      </c>
+      <c r="E99" s="137" t="s">
         <v>271</v>
       </c>
-      <c r="E99" s="137" t="s">
+      <c r="F99" s="137" t="s">
         <v>272</v>
-      </c>
-      <c r="F99" s="137" t="s">
-        <v>273</v>
       </c>
       <c r="G99" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H99" s="91" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I99" s="109">
         <v>24.18</v>
@@ -8235,13 +8232,13 @@
       </c>
       <c r="C100" s="132"/>
       <c r="D100" s="132" t="s">
+        <v>274</v>
+      </c>
+      <c r="E100" s="132" t="s">
         <v>275</v>
       </c>
-      <c r="E100" s="132" t="s">
+      <c r="F100" s="132" t="s">
         <v>276</v>
-      </c>
-      <c r="F100" s="132" t="s">
-        <v>277</v>
       </c>
       <c r="G100" s="94" t="s">
         <v>26</v>
@@ -8276,7 +8273,7 @@
         <v>1</v>
       </c>
       <c r="R100" s="127" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="101" ht="14" customHeight="1" spans="1:18">
@@ -8288,13 +8285,13 @@
       </c>
       <c r="C101" s="52"/>
       <c r="D101" s="53" t="s">
+        <v>277</v>
+      </c>
+      <c r="E101" s="53" t="s">
         <v>278</v>
       </c>
-      <c r="E101" s="53" t="s">
+      <c r="F101" s="53" t="s">
         <v>279</v>
-      </c>
-      <c r="F101" s="53" t="s">
-        <v>280</v>
       </c>
       <c r="G101" s="85" t="s">
         <v>26</v>
@@ -8341,16 +8338,16 @@
       </c>
       <c r="C102" s="47"/>
       <c r="D102" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E102" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="F102" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="E102" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="F102" s="47" t="s">
+      <c r="G102" s="85" t="s">
         <v>282</v>
-      </c>
-      <c r="G102" s="85" t="s">
-        <v>283</v>
       </c>
       <c r="H102" s="86" t="s">
         <v>38</v>
@@ -8380,7 +8377,7 @@
         <v>63</v>
       </c>
       <c r="R102" s="121" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" ht="12.75" customHeight="1" spans="1:18">
@@ -8392,19 +8389,19 @@
       </c>
       <c r="C103" s="60"/>
       <c r="D103" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="E103" s="61" t="s">
         <v>285</v>
       </c>
-      <c r="E103" s="61" t="s">
+      <c r="F103" s="61" t="s">
         <v>286</v>
-      </c>
-      <c r="F103" s="61" t="s">
-        <v>287</v>
       </c>
       <c r="G103" s="94" t="s">
         <v>26</v>
       </c>
       <c r="H103" s="95" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I103" s="113">
         <v>10.87</v>
@@ -8433,7 +8430,7 @@
         <v>10</v>
       </c>
       <c r="R103" s="127" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" ht="13" customHeight="1" spans="1:18">
@@ -8445,19 +8442,19 @@
       </c>
       <c r="C104" s="132"/>
       <c r="D104" s="132" t="s">
+        <v>288</v>
+      </c>
+      <c r="E104" s="132" t="s">
         <v>289</v>
       </c>
-      <c r="E104" s="132" t="s">
+      <c r="F104" s="132" t="s">
         <v>290</v>
-      </c>
-      <c r="F104" s="132" t="s">
-        <v>291</v>
       </c>
       <c r="G104" s="94" t="s">
         <v>26</v>
       </c>
       <c r="H104" s="95" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I104" s="113">
         <v>8.55</v>
@@ -8498,19 +8495,19 @@
       </c>
       <c r="C105" s="60"/>
       <c r="D105" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E105" s="61" t="s">
+        <v>285</v>
+      </c>
+      <c r="F105" s="61" t="s">
         <v>286</v>
-      </c>
-      <c r="F105" s="61" t="s">
-        <v>287</v>
       </c>
       <c r="G105" s="94" t="s">
         <v>26</v>
       </c>
       <c r="H105" s="95" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I105" s="113">
         <v>10.87</v>
@@ -8537,7 +8534,7 @@
         <v>0</v>
       </c>
       <c r="R105" s="127" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="106" ht="12" customHeight="1" spans="1:18">
@@ -8549,13 +8546,13 @@
       </c>
       <c r="C106" s="55"/>
       <c r="D106" s="55" t="s">
+        <v>294</v>
+      </c>
+      <c r="E106" s="55" t="s">
         <v>295</v>
       </c>
-      <c r="E106" s="55" t="s">
+      <c r="F106" s="55" t="s">
         <v>296</v>
-      </c>
-      <c r="F106" s="55" t="s">
-        <v>297</v>
       </c>
       <c r="G106" s="90" t="s">
         <v>26</v>
@@ -8598,19 +8595,19 @@
       </c>
       <c r="C107" s="49"/>
       <c r="D107" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="E107" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="E107" s="50" t="s">
+      <c r="F107" s="50" t="s">
         <v>299</v>
-      </c>
-      <c r="F107" s="50" t="s">
-        <v>300</v>
       </c>
       <c r="G107" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H107" s="88" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I107" s="107">
         <v>6.71</v>
@@ -8639,7 +8636,7 @@
         <v>14</v>
       </c>
       <c r="R107" s="122" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="108" ht="12.75" customHeight="1" spans="1:18">
@@ -8651,19 +8648,19 @@
       </c>
       <c r="C108" s="55"/>
       <c r="D108" s="55" t="s">
+        <v>302</v>
+      </c>
+      <c r="E108" s="55" t="s">
         <v>303</v>
       </c>
-      <c r="E108" s="55" t="s">
+      <c r="F108" s="55" t="s">
         <v>304</v>
-      </c>
-      <c r="F108" s="55" t="s">
-        <v>305</v>
       </c>
       <c r="G108" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H108" s="91" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I108" s="109">
         <v>7.97</v>
@@ -8692,7 +8689,7 @@
         <v>8</v>
       </c>
       <c r="R108" s="123" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="109" ht="12.75" customHeight="1" spans="1:18">
@@ -8704,19 +8701,19 @@
       </c>
       <c r="C109" s="52"/>
       <c r="D109" s="53" t="s">
+        <v>307</v>
+      </c>
+      <c r="E109" s="53" t="s">
         <v>308</v>
       </c>
-      <c r="E109" s="53" t="s">
+      <c r="F109" s="53" t="s">
         <v>309</v>
-      </c>
-      <c r="F109" s="53" t="s">
-        <v>310</v>
       </c>
       <c r="G109" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H109" s="86" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I109" s="105">
         <v>5.14</v>
@@ -8759,19 +8756,19 @@
       </c>
       <c r="C110" s="47"/>
       <c r="D110" s="47" t="s">
+        <v>311</v>
+      </c>
+      <c r="E110" s="47" t="s">
         <v>312</v>
       </c>
-      <c r="E110" s="47" t="s">
+      <c r="F110" s="47" t="s">
         <v>313</v>
-      </c>
-      <c r="F110" s="47" t="s">
-        <v>314</v>
       </c>
       <c r="G110" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H110" s="86" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I110" s="105">
         <v>51.06</v>
@@ -8814,13 +8811,13 @@
       </c>
       <c r="C111" s="52"/>
       <c r="D111" s="53" t="s">
+        <v>315</v>
+      </c>
+      <c r="E111" s="53" t="s">
         <v>316</v>
       </c>
-      <c r="E111" s="53" t="s">
-        <v>317</v>
-      </c>
       <c r="F111" s="53" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G111" s="85" t="s">
         <v>26</v>
@@ -8871,13 +8868,13 @@
       </c>
       <c r="C112" s="47"/>
       <c r="D112" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="E112" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="E112" s="47" t="s">
+      <c r="F112" s="47" t="s">
         <v>319</v>
-      </c>
-      <c r="F112" s="47" t="s">
-        <v>320</v>
       </c>
       <c r="G112" s="85" t="s">
         <v>26</v>
@@ -8926,13 +8923,13 @@
       </c>
       <c r="C113" s="60"/>
       <c r="D113" s="61" t="s">
+        <v>320</v>
+      </c>
+      <c r="E113" s="61" t="s">
+        <v>320</v>
+      </c>
+      <c r="F113" s="61" t="s">
         <v>321</v>
-      </c>
-      <c r="E113" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="F113" s="61" t="s">
-        <v>322</v>
       </c>
       <c r="G113" s="94" t="s">
         <v>26</v>
@@ -8967,7 +8964,7 @@
         <v>2</v>
       </c>
       <c r="R113" s="127" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="114" ht="13" customHeight="1" spans="1:18">
@@ -8979,19 +8976,19 @@
       </c>
       <c r="C114" s="130"/>
       <c r="D114" s="130" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E114" s="130" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F114" s="130" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G114" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H114" s="88" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I114" s="107">
         <v>5.87</v>
@@ -9028,13 +9025,13 @@
       </c>
       <c r="C115" s="60"/>
       <c r="D115" s="61" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E115" s="61" t="s">
         <v>145</v>
       </c>
       <c r="F115" s="61" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G115" s="94" t="s">
         <v>26</v>
@@ -9069,7 +9066,7 @@
         <v>2</v>
       </c>
       <c r="R115" s="125" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="116" ht="12" customHeight="1" spans="1:18">
@@ -9081,10 +9078,10 @@
       </c>
       <c r="C116" s="47"/>
       <c r="D116" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="E116" s="47" t="s">
         <v>329</v>
-      </c>
-      <c r="E116" s="47" t="s">
-        <v>330</v>
       </c>
       <c r="F116" s="47" t="s">
         <v>76</v>
@@ -9128,13 +9125,13 @@
       </c>
       <c r="C117" s="60"/>
       <c r="D117" s="61" t="s">
+        <v>330</v>
+      </c>
+      <c r="E117" s="61" t="s">
         <v>331</v>
       </c>
-      <c r="E117" s="61" t="s">
+      <c r="F117" s="61" t="s">
         <v>332</v>
-      </c>
-      <c r="F117" s="61" t="s">
-        <v>333</v>
       </c>
       <c r="G117" s="94" t="s">
         <v>26</v>
@@ -9167,7 +9164,7 @@
         <v>0</v>
       </c>
       <c r="R117" s="127" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="118" ht="13" customHeight="1" spans="1:18">
@@ -9179,19 +9176,19 @@
       </c>
       <c r="C118" s="55"/>
       <c r="D118" s="55" t="s">
+        <v>334</v>
+      </c>
+      <c r="E118" s="55" t="s">
+        <v>298</v>
+      </c>
+      <c r="F118" s="55" t="s">
         <v>335</v>
-      </c>
-      <c r="E118" s="55" t="s">
-        <v>299</v>
-      </c>
-      <c r="F118" s="55" t="s">
-        <v>336</v>
       </c>
       <c r="G118" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H118" s="91" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I118" s="109">
         <v>5.87</v>
@@ -9228,19 +9225,19 @@
       </c>
       <c r="C119" s="52"/>
       <c r="D119" s="53" t="s">
+        <v>336</v>
+      </c>
+      <c r="E119" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="F119" s="53" t="s">
         <v>337</v>
-      </c>
-      <c r="E119" s="53" t="s">
-        <v>317</v>
-      </c>
-      <c r="F119" s="53" t="s">
-        <v>338</v>
       </c>
       <c r="G119" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H119" s="86" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I119" s="105">
         <v>7.34</v>
@@ -9285,19 +9282,19 @@
       </c>
       <c r="C120" s="47"/>
       <c r="D120" s="47" t="s">
+        <v>339</v>
+      </c>
+      <c r="E120" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="E120" s="47" t="s">
+      <c r="F120" s="47" t="s">
         <v>341</v>
-      </c>
-      <c r="F120" s="47" t="s">
-        <v>342</v>
       </c>
       <c r="G120" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H120" s="86" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I120" s="105">
         <v>4.94</v>
@@ -9342,19 +9339,19 @@
       </c>
       <c r="C121" s="52"/>
       <c r="D121" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="E121" s="53" t="s">
         <v>344</v>
       </c>
-      <c r="E121" s="53" t="s">
+      <c r="F121" s="53" t="s">
         <v>345</v>
-      </c>
-      <c r="F121" s="53" t="s">
-        <v>346</v>
       </c>
       <c r="G121" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H121" s="86" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I121" s="105">
         <v>9.64</v>
@@ -9395,13 +9392,13 @@
       </c>
       <c r="C122" s="132"/>
       <c r="D122" s="132" t="s">
+        <v>347</v>
+      </c>
+      <c r="E122" s="132" t="s">
         <v>348</v>
       </c>
-      <c r="E122" s="132" t="s">
+      <c r="F122" s="132" t="s">
         <v>349</v>
-      </c>
-      <c r="F122" s="132" t="s">
-        <v>350</v>
       </c>
       <c r="G122" s="94" t="s">
         <v>127</v>
@@ -9432,7 +9429,7 @@
         <v>0</v>
       </c>
       <c r="R122" s="127" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="123" ht="12.75" customHeight="1" spans="1:18">
@@ -9443,16 +9440,16 @@
         <v>38</v>
       </c>
       <c r="C123" s="57" t="s">
+        <v>351</v>
+      </c>
+      <c r="D123" s="58" t="s">
         <v>352</v>
       </c>
-      <c r="D123" s="58" t="s">
+      <c r="E123" s="58" t="s">
         <v>353</v>
       </c>
-      <c r="E123" s="58" t="s">
+      <c r="F123" s="58" t="s">
         <v>354</v>
-      </c>
-      <c r="F123" s="58" t="s">
-        <v>355</v>
       </c>
       <c r="G123" s="92" t="s">
         <v>127</v>
@@ -9495,19 +9492,19 @@
       </c>
       <c r="C124" s="139"/>
       <c r="D124" s="139" t="s">
+        <v>355</v>
+      </c>
+      <c r="E124" s="139" t="s">
         <v>356</v>
       </c>
-      <c r="E124" s="139" t="s">
+      <c r="F124" s="139" t="s">
         <v>357</v>
-      </c>
-      <c r="F124" s="139" t="s">
-        <v>358</v>
       </c>
       <c r="G124" s="152" t="s">
         <v>26</v>
       </c>
       <c r="H124" s="91" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I124" s="109">
         <v>5.83</v>
@@ -9536,7 +9533,7 @@
         <v>2</v>
       </c>
       <c r="R124" s="123" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="125" ht="28" customHeight="1" spans="1:18">
@@ -9549,7 +9546,7 @@
       <c r="G125" s="153"/>
       <c r="H125" s="154"/>
       <c r="I125" s="162" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J125" s="163">
         <f>SUM(J6:J124)</f>
@@ -27163,7 +27160,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="5"/>
@@ -27223,7 +27220,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44673</v>
+        <v>44678</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -27250,13 +27247,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:26">
       <c r="A5" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>7</v>
@@ -27298,7 +27295,7 @@
         <v>0.1</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>23</v>
@@ -27340,7 +27337,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>23</v>
@@ -27382,7 +27379,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>23</v>
@@ -27424,7 +27421,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>23</v>
@@ -27466,7 +27463,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>23</v>
@@ -27505,10 +27502,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>370</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>371</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>23</v>
@@ -27517,7 +27514,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>26</v>
@@ -27550,7 +27547,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>23</v>
@@ -27592,7 +27589,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>23</v>
@@ -27634,7 +27631,7 @@
         <v>43</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>23</v>
@@ -27674,16 +27671,16 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>376</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="E15" s="12" t="s">
         <v>377</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>378</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>379</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>26</v>
@@ -27714,16 +27711,16 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>380</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>382</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>383</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>26</v>
@@ -27754,16 +27751,16 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>385</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>382</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>386</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>26</v>
@@ -27794,7 +27791,7 @@
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>94</v>
@@ -27834,16 +27831,16 @@
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>390</v>
-      </c>
       <c r="F19" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>26</v>
@@ -27874,16 +27871,16 @@
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>393</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>394</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>26</v>
@@ -27914,16 +27911,16 @@
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>397</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>398</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>26</v>
@@ -27954,16 +27951,16 @@
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>401</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>402</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>26</v>
@@ -27994,16 +27991,16 @@
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>404</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>405</v>
-      </c>
       <c r="F23" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>26</v>
@@ -28034,16 +28031,16 @@
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12" t="s">
+        <v>405</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="E24" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="F24" s="12" t="s">
         <v>408</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>409</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>26</v>
@@ -28074,13 +28071,13 @@
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>411</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>412</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>117</v>
@@ -28114,16 +28111,16 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="E26" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="F26" s="12" t="s">
         <v>415</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>416</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>26</v>
@@ -28154,16 +28151,16 @@
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>417</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="E27" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="F27" s="12" t="s">
         <v>419</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>420</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>26</v>
@@ -28194,16 +28191,16 @@
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>421</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="E28" s="12" t="s">
         <v>422</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="F28" s="12" t="s">
         <v>423</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>424</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>26</v>
@@ -28234,16 +28231,16 @@
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="E29" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="F29" s="12" t="s">
         <v>427</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>428</v>
       </c>
       <c r="G29" s="18" t="s">
         <v>26</v>
@@ -28274,7 +28271,7 @@
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>125</v>
@@ -28316,7 +28313,7 @@
         <v>120</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>121</v>
@@ -28355,10 +28352,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>431</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>432</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>133</v>
@@ -28367,7 +28364,7 @@
         <v>134</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>26</v>
@@ -28398,16 +28395,16 @@
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="E33" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>435</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>435</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>436</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>26</v>
@@ -28440,7 +28437,7 @@
         <v>100</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>164</v>
@@ -28482,7 +28479,7 @@
         <v>178</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>164</v>
@@ -28524,7 +28521,7 @@
         <v>3.01</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>164</v>
@@ -28533,7 +28530,7 @@
         <v>36</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>26</v>
@@ -28566,7 +28563,7 @@
         <v>205</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>164</v>
@@ -28608,7 +28605,7 @@
         <v>174</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>164</v>
@@ -28650,7 +28647,7 @@
         <v>199</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>164</v>
@@ -28692,7 +28689,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>164</v>
@@ -28734,7 +28731,7 @@
         <v>197</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>164</v>
@@ -28773,10 +28770,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>446</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>447</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>164</v>
@@ -28785,7 +28782,7 @@
         <v>36</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G42" s="18" t="s">
         <v>26</v>
@@ -28815,10 +28812,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>449</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>450</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>164</v>
@@ -28827,7 +28824,7 @@
         <v>36</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G43" s="18" t="s">
         <v>26</v>
@@ -28857,10 +28854,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="C44" s="12" t="s">
         <v>452</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>453</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>164</v>
@@ -28869,7 +28866,7 @@
         <v>36</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>26</v>
@@ -28902,7 +28899,7 @@
         <v>237</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>164</v>
@@ -28941,19 +28938,19 @@
         <v>8</v>
       </c>
       <c r="B46" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>456</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>457</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>164</v>
       </c>
       <c r="E46" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="F46" s="12" t="s">
         <v>458</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>459</v>
       </c>
       <c r="G46" s="18" t="s">
         <v>26</v>
@@ -28984,16 +28981,16 @@
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="E47" s="12" t="s">
         <v>461</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="F47" s="12" t="s">
         <v>462</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>463</v>
       </c>
       <c r="G47" s="18" t="s">
         <v>26</v>
@@ -29024,16 +29021,16 @@
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="E48" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="F48" s="12" t="s">
         <v>466</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>467</v>
       </c>
       <c r="G48" s="18" t="s">
         <v>26</v>
@@ -29064,16 +29061,16 @@
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D49" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="E49" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="F49" s="12" t="s">
         <v>304</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>305</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>26</v>
@@ -29104,16 +29101,16 @@
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="F50" s="12" t="s">
         <v>471</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>472</v>
       </c>
       <c r="G50" s="18" t="s">
         <v>26</v>
@@ -29144,16 +29141,16 @@
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="E51" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="F51" s="12" t="s">
         <v>475</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>476</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>26</v>
@@ -29184,16 +29181,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>478</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="F52" s="12" t="s">
         <v>479</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>480</v>
       </c>
       <c r="G52" s="18" t="s">
         <v>26</v>
@@ -29224,16 +29221,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>481</v>
       </c>
-      <c r="D53" s="12" t="s">
-        <v>482</v>
-      </c>
       <c r="E53" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G53" s="18" t="s">
         <v>26</v>
@@ -29264,16 +29261,16 @@
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G54" s="18" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
update some number of caps. Not enough for 32 quabos.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -1553,10 +1553,10 @@
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="178" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1668,28 +1668,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1705,9 +1691,32 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1720,7 +1729,75 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1735,84 +1812,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1902,7 +1902,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1920,7 +1944,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1932,109 +2028,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2052,37 +2046,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2492,6 +2492,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2516,13 +2531,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2544,187 +2563,168 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="13" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="38" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3424,10 +3424,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D71" activePane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D6" workbookViewId="0">
+      <pane ySplit="1170" topLeftCell="D20" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R95" sqref="R95"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="$A22:$XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3546,7 +3546,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44678</v>
+        <v>44679</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -3901,10 +3901,12 @@
       <c r="O12" s="104">
         <v>0</v>
       </c>
-      <c r="P12" s="104"/>
+      <c r="P12" s="104">
+        <v>185</v>
+      </c>
       <c r="Q12" s="104">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="R12" s="120"/>
     </row>
@@ -4235,10 +4237,12 @@
       <c r="O19" s="104">
         <v>0</v>
       </c>
-      <c r="P19" s="104"/>
+      <c r="P19" s="104">
+        <v>18</v>
+      </c>
       <c r="Q19" s="104">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R19" s="120"/>
     </row>
@@ -4916,12 +4920,9 @@
         <v>0</v>
       </c>
       <c r="P33" s="104">
-        <v>5</v>
-      </c>
-      <c r="Q33" s="104">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="Q33" s="104"/>
       <c r="R33" s="120"/>
     </row>
     <row r="34" customHeight="1" spans="1:18">
@@ -5445,10 +5446,12 @@
       <c r="O43" s="112" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="P43" s="112"/>
+      <c r="P43" s="112">
+        <v>30</v>
+      </c>
       <c r="Q43" s="112">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="R43" s="124"/>
     </row>
@@ -6024,10 +6027,12 @@
       <c r="O54" s="104">
         <v>0</v>
       </c>
-      <c r="P54" s="104"/>
+      <c r="P54" s="104">
+        <v>20</v>
+      </c>
       <c r="Q54" s="104">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R54" s="120"/>
     </row>
@@ -27220,7 +27225,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44678</v>
+        <v>44679</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
we received TFM connectors.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="483">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -1550,13 +1550,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="176" formatCode="[$-C09]dd\-mmm\-yy"/>
     <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1667,8 +1667,46 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1682,8 +1720,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1698,70 +1790,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1772,47 +1810,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1902,7 +1902,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1914,7 +1914,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1932,25 +1998,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1962,7 +2016,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1974,7 +2034,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1986,103 +2076,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2487,7 +2487,57 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2510,38 +2560,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2560,171 +2580,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2736,7 +2736,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2787,7 +2787,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2886,14 +2886,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2917,7 +2917,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2932,7 +2932,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2956,7 +2956,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3109,16 +3109,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3424,10 +3424,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D6" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
       <pane ySplit="1170" topLeftCell="D20" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="$A22:$XFD22"/>
+      <selection pane="bottomLeft" activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3546,7 +3546,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44679</v>
+        <v>44701</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -5235,7 +5235,7 @@
         <v>666.88</v>
       </c>
       <c r="N39" s="106">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O39" s="106">
         <v>666.88</v>
@@ -5243,9 +5243,11 @@
       <c r="P39" s="106"/>
       <c r="Q39" s="106">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R39" s="121"/>
+        <v>32</v>
+      </c>
+      <c r="R39" s="121" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="40" ht="12" customHeight="1" spans="1:18">
       <c r="A40" s="54">
@@ -27225,7 +27227,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44679</v>
+        <v>44701</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
received 7 VM53S3 from Lincoln.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -908,7 +908,7 @@
     <t>Dove</t>
   </si>
   <si>
-    <t>Dan have some</t>
+    <t>Dan have some. we also received 7 from Linclon.</t>
   </si>
   <si>
     <t>CDCM61004RHB</t>
@@ -1550,13 +1550,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="[$-C09]dd\-mmm\-yy"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1682,11 +1682,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1720,11 +1719,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1737,7 +1750,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1748,6 +1761,36 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1767,52 +1810,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1902,12 +1902,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1920,7 +1914,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1932,7 +1974,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1944,19 +1998,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1968,7 +2010,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1980,7 +2058,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1992,97 +2082,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2487,15 +2487,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2516,6 +2507,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2523,6 +2529,24 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2556,169 +2580,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="39" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2736,7 +2736,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2761,7 +2761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2787,7 +2787,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2886,14 +2886,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2917,7 +2917,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2932,7 +2932,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2956,61 +2956,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3109,16 +3109,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3145,16 +3145,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3425,9 +3425,9 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D20" activePane="bottomLeft"/>
+      <pane ySplit="1170" topLeftCell="D73" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="S39" sqref="S39"/>
+      <selection pane="bottomLeft" activeCell="R102" sqref="R102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3546,7 +3546,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44701</v>
+        <v>44705</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -8372,7 +8372,9 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N102" s="106"/>
+      <c r="N102" s="106">
+        <v>7</v>
+      </c>
       <c r="O102" s="106" t="e">
         <v>#VALUE!</v>
       </c>
@@ -8380,8 +8382,8 @@
         <v>63</v>
       </c>
       <c r="Q102" s="106">
-        <f t="shared" si="15"/>
-        <v>63</v>
+        <f>$N102+$P102</f>
+        <v>70</v>
       </c>
       <c r="R102" s="121" t="s">
         <v>283</v>
@@ -27227,7 +27229,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44701</v>
+        <v>44705</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
we received LT3022IMSE * 32.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="483">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -1550,13 +1550,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="[$-C09]dd\-mmm\-yy"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1683,29 +1683,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1720,15 +1720,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1743,14 +1735,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1764,8 +1749,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1773,7 +1766,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1788,33 +1804,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1902,7 +1902,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1914,7 +1920,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1926,37 +1938,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1974,7 +1956,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1992,7 +1992,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2010,13 +2034,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2028,19 +2046,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2052,37 +2076,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2487,7 +2487,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2507,6 +2507,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2518,6 +2527,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2542,30 +2566,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2583,142 +2583,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="39" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="37" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2736,7 +2736,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2761,7 +2761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2787,7 +2787,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2886,14 +2886,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2917,7 +2917,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2932,7 +2932,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2956,61 +2956,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3109,16 +3109,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3145,16 +3145,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3425,9 +3425,9 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D73" activePane="bottomLeft"/>
+      <pane ySplit="1170" topLeftCell="D86" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R102" sqref="R102"/>
+      <selection pane="bottomLeft" activeCell="R121" sqref="R121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3546,7 +3546,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44705</v>
+        <v>44706</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -8382,7 +8382,7 @@
         <v>63</v>
       </c>
       <c r="Q102" s="106">
-        <f>$N102+$P102</f>
+        <f t="shared" si="15"/>
         <v>70</v>
       </c>
       <c r="R102" s="121" t="s">
@@ -9380,7 +9380,7 @@
         <v>308.48</v>
       </c>
       <c r="N121" s="106">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O121" s="106">
         <v>308.48</v>
@@ -9388,9 +9388,11 @@
       <c r="P121" s="106"/>
       <c r="Q121" s="106">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R121" s="121"/>
+        <v>32</v>
+      </c>
+      <c r="R121" s="121" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="122" ht="13" customHeight="1" spans="1:18">
       <c r="A122" s="131">
@@ -27229,7 +27231,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44705</v>
+        <v>44706</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
received DMMT3904W-FDICT-ND * 128.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="482">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -512,9 +512,6 @@
     <t>7/14/2022</t>
   </si>
   <si>
-    <t>Mouser Expected 4/29/2022 Update: same than digikey</t>
-  </si>
-  <si>
     <t>BF622</t>
   </si>
   <si>
@@ -1550,13 +1547,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1675,8 +1672,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1696,11 +1702,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1719,25 +1746,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1746,6 +1759,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1758,10 +1779,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1779,15 +1800,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1795,26 +1807,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1902,7 +1899,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1914,13 +1947,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1932,55 +1971,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1998,13 +1995,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2016,19 +2007,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2040,7 +2037,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2052,37 +2079,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2483,11 +2480,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2511,22 +2523,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2548,17 +2556,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -2566,162 +2563,162 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="37" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2736,7 +2733,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2761,7 +2758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2787,7 +2784,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2886,14 +2883,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2917,7 +2914,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2932,7 +2929,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2956,61 +2953,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3109,16 +3106,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3145,16 +3142,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3425,9 +3422,9 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D86" activePane="bottomLeft"/>
+      <pane ySplit="1170" topLeftCell="D30" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R121" sqref="R121"/>
+      <selection pane="bottomLeft" activeCell="R49" sqref="R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3546,7 +3543,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44706</v>
+        <v>44728</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -5767,7 +5764,7 @@
         <v>49.92</v>
       </c>
       <c r="N49" s="106">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="O49" s="106">
         <v>199.68</v>
@@ -5775,10 +5772,10 @@
       <c r="P49" s="106"/>
       <c r="Q49" s="106">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="R49" s="126" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" ht="12.75" customHeight="1" spans="1:18">
@@ -5790,19 +5787,19 @@
       </c>
       <c r="C50" s="47"/>
       <c r="D50" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="E50" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="E50" s="47" t="s">
+      <c r="F50" s="47" t="s">
         <v>153</v>
-      </c>
-      <c r="F50" s="47" t="s">
-        <v>154</v>
       </c>
       <c r="G50" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H50" s="86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I50" s="105">
         <v>0.44</v>
@@ -5847,13 +5844,13 @@
       </c>
       <c r="C51" s="60"/>
       <c r="D51" s="61" t="s">
+        <v>155</v>
+      </c>
+      <c r="E51" s="61" t="s">
         <v>156</v>
       </c>
-      <c r="E51" s="61" t="s">
+      <c r="F51" s="61" t="s">
         <v>157</v>
-      </c>
-      <c r="F51" s="61" t="s">
-        <v>158</v>
       </c>
       <c r="G51" s="94" t="s">
         <v>127</v>
@@ -5884,7 +5881,7 @@
         <v>0</v>
       </c>
       <c r="R51" s="127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" ht="14" customHeight="1" spans="1:18">
@@ -5896,13 +5893,13 @@
       </c>
       <c r="C52" s="63"/>
       <c r="D52" s="63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="63" t="s">
         <v>145</v>
       </c>
       <c r="F52" s="63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G52" s="96" t="s">
         <v>26</v>
@@ -5937,7 +5934,7 @@
         <v>9</v>
       </c>
       <c r="R52" s="128" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" ht="12" customHeight="1" spans="1:18">
@@ -5945,23 +5942,23 @@
         <v>8</v>
       </c>
       <c r="B53" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C53" s="42"/>
       <c r="D53" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E53" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F53" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G53" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H53" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I53" s="103"/>
       <c r="J53" s="103">
@@ -5993,17 +5990,17 @@
         <v>3</v>
       </c>
       <c r="B54" s="45" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C54" s="45"/>
       <c r="D54" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E54" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="F54" s="45" t="s">
         <v>168</v>
-      </c>
-      <c r="F54" s="45" t="s">
-        <v>169</v>
       </c>
       <c r="G54" s="82" t="s">
         <v>26</v>
@@ -6043,17 +6040,17 @@
         <v>1</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C55" s="42"/>
       <c r="D55" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E55" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F55" s="43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G55" s="82" t="s">
         <v>26</v>
@@ -6091,17 +6088,17 @@
         <v>1</v>
       </c>
       <c r="B56" s="45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C56" s="45"/>
       <c r="D56" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E56" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F56" s="45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G56" s="82" t="s">
         <v>26</v>
@@ -6143,7 +6140,7 @@
       </c>
       <c r="C57" s="52"/>
       <c r="D57" s="53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E57" s="53" t="s">
         <v>36</v>
@@ -6186,23 +6183,23 @@
         <v>16</v>
       </c>
       <c r="B58" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C58" s="45"/>
       <c r="D58" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E58" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F58" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G58" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H58" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I58" s="103"/>
       <c r="J58" s="103">
@@ -6234,17 +6231,17 @@
         <v>15</v>
       </c>
       <c r="B59" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C59" s="42"/>
       <c r="D59" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E59" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F59" s="43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G59" s="82" t="s">
         <v>26</v>
@@ -6282,23 +6279,23 @@
         <v>14</v>
       </c>
       <c r="B60" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C60" s="45"/>
       <c r="D60" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E60" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F60" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G60" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H60" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I60" s="103"/>
       <c r="J60" s="103">
@@ -6330,17 +6327,17 @@
         <v>4</v>
       </c>
       <c r="B61" s="42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C61" s="42"/>
       <c r="D61" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E61" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F61" s="43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G61" s="82" t="s">
         <v>26</v>
@@ -6378,17 +6375,17 @@
         <v>4</v>
       </c>
       <c r="B62" s="45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C62" s="45"/>
       <c r="D62" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E62" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F62" s="45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G62" s="82" t="s">
         <v>26</v>
@@ -6426,17 +6423,17 @@
         <v>8</v>
       </c>
       <c r="B63" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C63" s="42"/>
       <c r="D63" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E63" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F63" s="43" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G63" s="82" t="s">
         <v>26</v>
@@ -6474,17 +6471,17 @@
         <v>5</v>
       </c>
       <c r="B64" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C64" s="45"/>
       <c r="D64" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E64" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F64" s="45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G64" s="82" t="s">
         <v>26</v>
@@ -6522,17 +6519,17 @@
         <v>1</v>
       </c>
       <c r="B65" s="42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C65" s="42"/>
       <c r="D65" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E65" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F65" s="43" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G65" s="82" t="s">
         <v>26</v>
@@ -6570,17 +6567,17 @@
         <v>8</v>
       </c>
       <c r="B66" s="45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" s="45"/>
       <c r="D66" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E66" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F66" s="45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G66" s="82" t="s">
         <v>26</v>
@@ -6618,17 +6615,17 @@
         <v>4</v>
       </c>
       <c r="B67" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C67" s="42"/>
       <c r="D67" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E67" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F67" s="43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G67" s="82" t="s">
         <v>26</v>
@@ -6666,23 +6663,23 @@
         <v>5</v>
       </c>
       <c r="B68" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C68" s="45"/>
       <c r="D68" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E68" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F68" s="45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G68" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H68" s="83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I68" s="103"/>
       <c r="J68" s="103">
@@ -6714,17 +6711,17 @@
         <v>8</v>
       </c>
       <c r="B69" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C69" s="42"/>
       <c r="D69" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E69" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F69" s="43" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G69" s="82" t="s">
         <v>26</v>
@@ -6762,17 +6759,17 @@
         <v>1</v>
       </c>
       <c r="B70" s="45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C70" s="45"/>
       <c r="D70" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E70" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F70" s="45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G70" s="82" t="s">
         <v>26</v>
@@ -6810,17 +6807,17 @@
         <v>1</v>
       </c>
       <c r="B71" s="42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C71" s="42"/>
       <c r="D71" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E71" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F71" s="43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G71" s="82" t="s">
         <v>26</v>
@@ -6858,17 +6855,17 @@
         <v>3</v>
       </c>
       <c r="B72" s="45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C72" s="45"/>
       <c r="D72" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E72" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F72" s="45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G72" s="82" t="s">
         <v>26</v>
@@ -6906,23 +6903,23 @@
         <v>17</v>
       </c>
       <c r="B73" s="42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C73" s="42"/>
       <c r="D73" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E73" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F73" s="43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G73" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H73" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I73" s="103"/>
       <c r="J73" s="103">
@@ -6954,17 +6951,17 @@
         <v>3</v>
       </c>
       <c r="B74" s="45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C74" s="45"/>
       <c r="D74" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E74" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F74" s="45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G74" s="82" t="s">
         <v>26</v>
@@ -7002,17 +6999,17 @@
         <v>1</v>
       </c>
       <c r="B75" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C75" s="42"/>
       <c r="D75" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E75" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F75" s="43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G75" s="82" t="s">
         <v>26</v>
@@ -7050,17 +7047,17 @@
         <v>11</v>
       </c>
       <c r="B76" s="45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C76" s="45"/>
       <c r="D76" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E76" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F76" s="45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G76" s="82" t="s">
         <v>26</v>
@@ -7098,23 +7095,23 @@
         <v>6</v>
       </c>
       <c r="B77" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C77" s="42"/>
       <c r="D77" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E77" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F77" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G77" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H77" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I77" s="103"/>
       <c r="J77" s="103">
@@ -7146,17 +7143,17 @@
         <v>1</v>
       </c>
       <c r="B78" s="45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C78" s="45"/>
       <c r="D78" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E78" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F78" s="45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G78" s="82" t="s">
         <v>26</v>
@@ -7194,23 +7191,23 @@
         <v>2</v>
       </c>
       <c r="B79" s="42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C79" s="42"/>
       <c r="D79" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E79" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F79" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G79" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H79" s="83" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I79" s="103"/>
       <c r="J79" s="103">
@@ -7242,17 +7239,17 @@
         <v>1</v>
       </c>
       <c r="B80" s="45" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C80" s="45"/>
       <c r="D80" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E80" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F80" s="45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G80" s="82" t="s">
         <v>26</v>
@@ -7290,23 +7287,23 @@
         <v>1</v>
       </c>
       <c r="B81" s="42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C81" s="42"/>
       <c r="D81" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E81" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F81" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G81" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H81" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I81" s="103"/>
       <c r="J81" s="103">
@@ -7338,17 +7335,17 @@
         <v>1</v>
       </c>
       <c r="B82" s="45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C82" s="45"/>
       <c r="D82" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E82" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F82" s="45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G82" s="82" t="s">
         <v>26</v>
@@ -7386,17 +7383,17 @@
         <v>1</v>
       </c>
       <c r="B83" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C83" s="42"/>
       <c r="D83" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E83" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F83" s="43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G83" s="82" t="s">
         <v>26</v>
@@ -7434,17 +7431,17 @@
         <v>4</v>
       </c>
       <c r="B84" s="45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C84" s="45"/>
       <c r="D84" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E84" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F84" s="45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G84" s="82" t="s">
         <v>26</v>
@@ -7482,17 +7479,17 @@
         <v>4</v>
       </c>
       <c r="B85" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C85" s="42"/>
       <c r="D85" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E85" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F85" s="43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G85" s="82" t="s">
         <v>26</v>
@@ -7530,17 +7527,17 @@
         <v>2</v>
       </c>
       <c r="B86" s="45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C86" s="45"/>
       <c r="D86" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E86" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F86" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G86" s="82" t="s">
         <v>26</v>
@@ -7578,17 +7575,17 @@
         <v>2</v>
       </c>
       <c r="B87" s="42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C87" s="42"/>
       <c r="D87" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E87" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F87" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G87" s="82" t="s">
         <v>26</v>
@@ -7626,23 +7623,23 @@
         <v>1</v>
       </c>
       <c r="B88" s="45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C88" s="45"/>
       <c r="D88" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E88" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F88" s="45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G88" s="82" t="s">
         <v>26</v>
       </c>
       <c r="H88" s="83" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I88" s="103"/>
       <c r="J88" s="103">
@@ -7674,17 +7671,17 @@
         <v>1</v>
       </c>
       <c r="B89" s="42" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C89" s="42"/>
       <c r="D89" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E89" s="43" t="s">
         <v>36</v>
       </c>
       <c r="F89" s="43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G89" s="82" t="s">
         <v>26</v>
@@ -7722,17 +7719,17 @@
         <v>1</v>
       </c>
       <c r="B90" s="45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C90" s="45"/>
       <c r="D90" s="45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E90" s="45" t="s">
         <v>36</v>
       </c>
       <c r="F90" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G90" s="82" t="s">
         <v>26</v>
@@ -7770,17 +7767,17 @@
         <v>256</v>
       </c>
       <c r="B91" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C91" s="42"/>
       <c r="D91" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E91" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="F91" s="43" t="s">
         <v>243</v>
-      </c>
-      <c r="F91" s="43" t="s">
-        <v>244</v>
       </c>
       <c r="G91" s="82" t="s">
         <v>26</v>
@@ -7822,10 +7819,10 @@
       </c>
       <c r="C92" s="47"/>
       <c r="D92" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="E92" s="47" t="s">
         <v>245</v>
-      </c>
-      <c r="E92" s="47" t="s">
-        <v>246</v>
       </c>
       <c r="F92" s="47" t="s">
         <v>77</v>
@@ -7869,16 +7866,16 @@
       </c>
       <c r="C93" s="42"/>
       <c r="D93" s="43" t="s">
+        <v>246</v>
+      </c>
+      <c r="E93" s="43" t="s">
         <v>247</v>
-      </c>
-      <c r="E93" s="43" t="s">
-        <v>248</v>
       </c>
       <c r="F93" s="43" t="s">
         <v>38</v>
       </c>
       <c r="G93" s="82" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H93" s="83" t="s">
         <v>38</v>
@@ -7909,7 +7906,7 @@
         <v>20</v>
       </c>
       <c r="R93" s="120" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="94" ht="12" customHeight="1" spans="1:18">
@@ -7921,19 +7918,19 @@
       </c>
       <c r="C94" s="130"/>
       <c r="D94" s="130" t="s">
+        <v>250</v>
+      </c>
+      <c r="E94" s="130" t="s">
         <v>251</v>
       </c>
-      <c r="E94" s="130" t="s">
+      <c r="F94" s="130" t="s">
         <v>252</v>
-      </c>
-      <c r="F94" s="130" t="s">
-        <v>253</v>
       </c>
       <c r="G94" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H94" s="88" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I94" s="107">
         <v>599.2</v>
@@ -7970,19 +7967,19 @@
       </c>
       <c r="C95" s="52"/>
       <c r="D95" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="E95" s="53" t="s">
         <v>255</v>
       </c>
-      <c r="E95" s="53" t="s">
+      <c r="F95" s="53" t="s">
         <v>256</v>
-      </c>
-      <c r="F95" s="53" t="s">
-        <v>257</v>
       </c>
       <c r="G95" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H95" s="86" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I95" s="105">
         <v>9.23</v>
@@ -8027,13 +8024,13 @@
       </c>
       <c r="C96" s="132"/>
       <c r="D96" s="132" t="s">
+        <v>258</v>
+      </c>
+      <c r="E96" s="132" t="s">
         <v>259</v>
       </c>
-      <c r="E96" s="132" t="s">
+      <c r="F96" s="132" t="s">
         <v>260</v>
-      </c>
-      <c r="F96" s="132" t="s">
-        <v>261</v>
       </c>
       <c r="G96" s="94" t="s">
         <v>26</v>
@@ -8068,7 +8065,7 @@
         <v>1</v>
       </c>
       <c r="R96" s="127" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="97" ht="12.75" customHeight="1" spans="1:18">
@@ -8080,13 +8077,13 @@
       </c>
       <c r="C97" s="52"/>
       <c r="D97" s="53" t="s">
+        <v>262</v>
+      </c>
+      <c r="E97" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="E97" s="53" t="s">
+      <c r="F97" s="53" t="s">
         <v>264</v>
-      </c>
-      <c r="F97" s="53" t="s">
-        <v>265</v>
       </c>
       <c r="G97" s="85" t="s">
         <v>26</v>
@@ -8137,13 +8134,13 @@
       </c>
       <c r="C98" s="134"/>
       <c r="D98" s="134" t="s">
+        <v>265</v>
+      </c>
+      <c r="E98" s="134" t="s">
         <v>266</v>
       </c>
-      <c r="E98" s="134" t="s">
+      <c r="F98" s="134" t="s">
         <v>267</v>
-      </c>
-      <c r="F98" s="134" t="s">
-        <v>268</v>
       </c>
       <c r="G98" s="149" t="s">
         <v>26</v>
@@ -8178,7 +8175,7 @@
         <v>2</v>
       </c>
       <c r="R98" s="165" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99" ht="14" customHeight="1" spans="1:18">
@@ -8190,19 +8187,19 @@
       </c>
       <c r="C99" s="136"/>
       <c r="D99" s="137" t="s">
+        <v>269</v>
+      </c>
+      <c r="E99" s="137" t="s">
         <v>270</v>
       </c>
-      <c r="E99" s="137" t="s">
+      <c r="F99" s="137" t="s">
         <v>271</v>
-      </c>
-      <c r="F99" s="137" t="s">
-        <v>272</v>
       </c>
       <c r="G99" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H99" s="91" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I99" s="109">
         <v>24.18</v>
@@ -8239,13 +8236,13 @@
       </c>
       <c r="C100" s="132"/>
       <c r="D100" s="132" t="s">
+        <v>273</v>
+      </c>
+      <c r="E100" s="132" t="s">
         <v>274</v>
       </c>
-      <c r="E100" s="132" t="s">
+      <c r="F100" s="132" t="s">
         <v>275</v>
-      </c>
-      <c r="F100" s="132" t="s">
-        <v>276</v>
       </c>
       <c r="G100" s="94" t="s">
         <v>26</v>
@@ -8280,7 +8277,7 @@
         <v>1</v>
       </c>
       <c r="R100" s="127" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="101" ht="14" customHeight="1" spans="1:18">
@@ -8292,13 +8289,13 @@
       </c>
       <c r="C101" s="52"/>
       <c r="D101" s="53" t="s">
+        <v>276</v>
+      </c>
+      <c r="E101" s="53" t="s">
         <v>277</v>
       </c>
-      <c r="E101" s="53" t="s">
+      <c r="F101" s="53" t="s">
         <v>278</v>
-      </c>
-      <c r="F101" s="53" t="s">
-        <v>279</v>
       </c>
       <c r="G101" s="85" t="s">
         <v>26</v>
@@ -8345,16 +8342,16 @@
       </c>
       <c r="C102" s="47"/>
       <c r="D102" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="E102" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="F102" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="E102" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="F102" s="47" t="s">
+      <c r="G102" s="85" t="s">
         <v>281</v>
-      </c>
-      <c r="G102" s="85" t="s">
-        <v>282</v>
       </c>
       <c r="H102" s="86" t="s">
         <v>38</v>
@@ -8386,7 +8383,7 @@
         <v>70</v>
       </c>
       <c r="R102" s="121" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" ht="12.75" customHeight="1" spans="1:18">
@@ -8398,19 +8395,19 @@
       </c>
       <c r="C103" s="60"/>
       <c r="D103" s="61" t="s">
+        <v>283</v>
+      </c>
+      <c r="E103" s="61" t="s">
         <v>284</v>
       </c>
-      <c r="E103" s="61" t="s">
+      <c r="F103" s="61" t="s">
         <v>285</v>
-      </c>
-      <c r="F103" s="61" t="s">
-        <v>286</v>
       </c>
       <c r="G103" s="94" t="s">
         <v>26</v>
       </c>
       <c r="H103" s="95" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I103" s="113">
         <v>10.87</v>
@@ -8439,7 +8436,7 @@
         <v>10</v>
       </c>
       <c r="R103" s="127" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" ht="13" customHeight="1" spans="1:18">
@@ -8451,19 +8448,19 @@
       </c>
       <c r="C104" s="132"/>
       <c r="D104" s="132" t="s">
+        <v>287</v>
+      </c>
+      <c r="E104" s="132" t="s">
         <v>288</v>
       </c>
-      <c r="E104" s="132" t="s">
+      <c r="F104" s="132" t="s">
         <v>289</v>
-      </c>
-      <c r="F104" s="132" t="s">
-        <v>290</v>
       </c>
       <c r="G104" s="94" t="s">
         <v>26</v>
       </c>
       <c r="H104" s="95" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I104" s="113">
         <v>8.55</v>
@@ -8492,7 +8489,7 @@
         <v>1</v>
       </c>
       <c r="R104" s="127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="105" ht="13" customHeight="1" spans="1:18">
@@ -8504,19 +8501,19 @@
       </c>
       <c r="C105" s="60"/>
       <c r="D105" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E105" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="F105" s="61" t="s">
         <v>285</v>
-      </c>
-      <c r="F105" s="61" t="s">
-        <v>286</v>
       </c>
       <c r="G105" s="94" t="s">
         <v>26</v>
       </c>
       <c r="H105" s="95" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I105" s="113">
         <v>10.87</v>
@@ -8543,7 +8540,7 @@
         <v>0</v>
       </c>
       <c r="R105" s="127" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" ht="12" customHeight="1" spans="1:18">
@@ -8555,13 +8552,13 @@
       </c>
       <c r="C106" s="55"/>
       <c r="D106" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="E106" s="55" t="s">
         <v>294</v>
       </c>
-      <c r="E106" s="55" t="s">
+      <c r="F106" s="55" t="s">
         <v>295</v>
-      </c>
-      <c r="F106" s="55" t="s">
-        <v>296</v>
       </c>
       <c r="G106" s="90" t="s">
         <v>26</v>
@@ -8604,19 +8601,19 @@
       </c>
       <c r="C107" s="49"/>
       <c r="D107" s="50" t="s">
+        <v>296</v>
+      </c>
+      <c r="E107" s="50" t="s">
         <v>297</v>
       </c>
-      <c r="E107" s="50" t="s">
+      <c r="F107" s="50" t="s">
         <v>298</v>
-      </c>
-      <c r="F107" s="50" t="s">
-        <v>299</v>
       </c>
       <c r="G107" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H107" s="88" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I107" s="107">
         <v>6.71</v>
@@ -8645,7 +8642,7 @@
         <v>14</v>
       </c>
       <c r="R107" s="122" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="108" ht="12.75" customHeight="1" spans="1:18">
@@ -8657,19 +8654,19 @@
       </c>
       <c r="C108" s="55"/>
       <c r="D108" s="55" t="s">
+        <v>301</v>
+      </c>
+      <c r="E108" s="55" t="s">
         <v>302</v>
       </c>
-      <c r="E108" s="55" t="s">
+      <c r="F108" s="55" t="s">
         <v>303</v>
-      </c>
-      <c r="F108" s="55" t="s">
-        <v>304</v>
       </c>
       <c r="G108" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H108" s="91" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I108" s="109">
         <v>7.97</v>
@@ -8698,7 +8695,7 @@
         <v>8</v>
       </c>
       <c r="R108" s="123" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="109" ht="12.75" customHeight="1" spans="1:18">
@@ -8710,19 +8707,19 @@
       </c>
       <c r="C109" s="52"/>
       <c r="D109" s="53" t="s">
+        <v>306</v>
+      </c>
+      <c r="E109" s="53" t="s">
         <v>307</v>
       </c>
-      <c r="E109" s="53" t="s">
+      <c r="F109" s="53" t="s">
         <v>308</v>
-      </c>
-      <c r="F109" s="53" t="s">
-        <v>309</v>
       </c>
       <c r="G109" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H109" s="86" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I109" s="105">
         <v>5.14</v>
@@ -8765,19 +8762,19 @@
       </c>
       <c r="C110" s="47"/>
       <c r="D110" s="47" t="s">
+        <v>310</v>
+      </c>
+      <c r="E110" s="47" t="s">
         <v>311</v>
       </c>
-      <c r="E110" s="47" t="s">
+      <c r="F110" s="47" t="s">
         <v>312</v>
-      </c>
-      <c r="F110" s="47" t="s">
-        <v>313</v>
       </c>
       <c r="G110" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H110" s="86" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I110" s="105">
         <v>51.06</v>
@@ -8820,13 +8817,13 @@
       </c>
       <c r="C111" s="52"/>
       <c r="D111" s="53" t="s">
+        <v>314</v>
+      </c>
+      <c r="E111" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="E111" s="53" t="s">
-        <v>316</v>
-      </c>
       <c r="F111" s="53" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G111" s="85" t="s">
         <v>26</v>
@@ -8877,13 +8874,13 @@
       </c>
       <c r="C112" s="47"/>
       <c r="D112" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="E112" s="47" t="s">
         <v>317</v>
       </c>
-      <c r="E112" s="47" t="s">
+      <c r="F112" s="47" t="s">
         <v>318</v>
-      </c>
-      <c r="F112" s="47" t="s">
-        <v>319</v>
       </c>
       <c r="G112" s="85" t="s">
         <v>26</v>
@@ -8932,13 +8929,13 @@
       </c>
       <c r="C113" s="60"/>
       <c r="D113" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="E113" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="F113" s="61" t="s">
         <v>320</v>
-      </c>
-      <c r="E113" s="61" t="s">
-        <v>320</v>
-      </c>
-      <c r="F113" s="61" t="s">
-        <v>321</v>
       </c>
       <c r="G113" s="94" t="s">
         <v>26</v>
@@ -8973,7 +8970,7 @@
         <v>2</v>
       </c>
       <c r="R113" s="127" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" ht="13" customHeight="1" spans="1:18">
@@ -8985,19 +8982,19 @@
       </c>
       <c r="C114" s="130"/>
       <c r="D114" s="130" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E114" s="130" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F114" s="130" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G114" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H114" s="88" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I114" s="107">
         <v>5.87</v>
@@ -9034,13 +9031,13 @@
       </c>
       <c r="C115" s="60"/>
       <c r="D115" s="61" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E115" s="61" t="s">
         <v>145</v>
       </c>
       <c r="F115" s="61" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G115" s="94" t="s">
         <v>26</v>
@@ -9075,7 +9072,7 @@
         <v>2</v>
       </c>
       <c r="R115" s="125" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116" ht="12" customHeight="1" spans="1:18">
@@ -9087,10 +9084,10 @@
       </c>
       <c r="C116" s="47"/>
       <c r="D116" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="E116" s="47" t="s">
         <v>328</v>
-      </c>
-      <c r="E116" s="47" t="s">
-        <v>329</v>
       </c>
       <c r="F116" s="47" t="s">
         <v>76</v>
@@ -9134,13 +9131,13 @@
       </c>
       <c r="C117" s="60"/>
       <c r="D117" s="61" t="s">
+        <v>329</v>
+      </c>
+      <c r="E117" s="61" t="s">
         <v>330</v>
       </c>
-      <c r="E117" s="61" t="s">
+      <c r="F117" s="61" t="s">
         <v>331</v>
-      </c>
-      <c r="F117" s="61" t="s">
-        <v>332</v>
       </c>
       <c r="G117" s="94" t="s">
         <v>26</v>
@@ -9173,7 +9170,7 @@
         <v>0</v>
       </c>
       <c r="R117" s="127" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" ht="13" customHeight="1" spans="1:18">
@@ -9185,19 +9182,19 @@
       </c>
       <c r="C118" s="55"/>
       <c r="D118" s="55" t="s">
+        <v>333</v>
+      </c>
+      <c r="E118" s="55" t="s">
+        <v>297</v>
+      </c>
+      <c r="F118" s="55" t="s">
         <v>334</v>
-      </c>
-      <c r="E118" s="55" t="s">
-        <v>298</v>
-      </c>
-      <c r="F118" s="55" t="s">
-        <v>335</v>
       </c>
       <c r="G118" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H118" s="91" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I118" s="109">
         <v>5.87</v>
@@ -9234,19 +9231,19 @@
       </c>
       <c r="C119" s="52"/>
       <c r="D119" s="53" t="s">
+        <v>335</v>
+      </c>
+      <c r="E119" s="53" t="s">
+        <v>315</v>
+      </c>
+      <c r="F119" s="53" t="s">
         <v>336</v>
-      </c>
-      <c r="E119" s="53" t="s">
-        <v>316</v>
-      </c>
-      <c r="F119" s="53" t="s">
-        <v>337</v>
       </c>
       <c r="G119" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H119" s="86" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I119" s="105">
         <v>7.34</v>
@@ -9291,19 +9288,19 @@
       </c>
       <c r="C120" s="47"/>
       <c r="D120" s="47" t="s">
+        <v>338</v>
+      </c>
+      <c r="E120" s="47" t="s">
         <v>339</v>
       </c>
-      <c r="E120" s="47" t="s">
+      <c r="F120" s="47" t="s">
         <v>340</v>
-      </c>
-      <c r="F120" s="47" t="s">
-        <v>341</v>
       </c>
       <c r="G120" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H120" s="86" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I120" s="105">
         <v>4.94</v>
@@ -9348,19 +9345,19 @@
       </c>
       <c r="C121" s="52"/>
       <c r="D121" s="53" t="s">
+        <v>342</v>
+      </c>
+      <c r="E121" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="E121" s="53" t="s">
+      <c r="F121" s="53" t="s">
         <v>344</v>
-      </c>
-      <c r="F121" s="53" t="s">
-        <v>345</v>
       </c>
       <c r="G121" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H121" s="86" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I121" s="105">
         <v>9.64</v>
@@ -9403,13 +9400,13 @@
       </c>
       <c r="C122" s="132"/>
       <c r="D122" s="132" t="s">
+        <v>346</v>
+      </c>
+      <c r="E122" s="132" t="s">
         <v>347</v>
       </c>
-      <c r="E122" s="132" t="s">
+      <c r="F122" s="132" t="s">
         <v>348</v>
-      </c>
-      <c r="F122" s="132" t="s">
-        <v>349</v>
       </c>
       <c r="G122" s="94" t="s">
         <v>127</v>
@@ -9440,7 +9437,7 @@
         <v>0</v>
       </c>
       <c r="R122" s="127" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="123" ht="12.75" customHeight="1" spans="1:18">
@@ -9451,16 +9448,16 @@
         <v>38</v>
       </c>
       <c r="C123" s="57" t="s">
+        <v>350</v>
+      </c>
+      <c r="D123" s="58" t="s">
         <v>351</v>
       </c>
-      <c r="D123" s="58" t="s">
+      <c r="E123" s="58" t="s">
         <v>352</v>
       </c>
-      <c r="E123" s="58" t="s">
+      <c r="F123" s="58" t="s">
         <v>353</v>
-      </c>
-      <c r="F123" s="58" t="s">
-        <v>354</v>
       </c>
       <c r="G123" s="92" t="s">
         <v>127</v>
@@ -9503,19 +9500,19 @@
       </c>
       <c r="C124" s="139"/>
       <c r="D124" s="139" t="s">
+        <v>354</v>
+      </c>
+      <c r="E124" s="139" t="s">
         <v>355</v>
       </c>
-      <c r="E124" s="139" t="s">
+      <c r="F124" s="139" t="s">
         <v>356</v>
-      </c>
-      <c r="F124" s="139" t="s">
-        <v>357</v>
       </c>
       <c r="G124" s="152" t="s">
         <v>26</v>
       </c>
       <c r="H124" s="91" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I124" s="109">
         <v>5.83</v>
@@ -9544,7 +9541,7 @@
         <v>2</v>
       </c>
       <c r="R124" s="123" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="125" ht="28" customHeight="1" spans="1:18">
@@ -9557,7 +9554,7 @@
       <c r="G125" s="153"/>
       <c r="H125" s="154"/>
       <c r="I125" s="162" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J125" s="163">
         <f>SUM(J6:J124)</f>
@@ -27102,7 +27099,7 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="Quabo_BGA.PrjPcb&#10;From:17.08.DN001.v06_Quabo_BOM"/>
     <hyperlink ref="R47" r:id="rId2" display="From Mouser"/>
-    <hyperlink ref="R49" r:id="rId3" display="Mouser Expected 4/29/2022 Update: same than digikey"/>
+    <hyperlink ref="R49" r:id="rId3" display="RAL Dig Lab"/>
     <hyperlink ref="R51" r:id="rId4" display="Rochester"/>
     <hyperlink ref="R96" r:id="rId5" display="Winsource"/>
     <hyperlink ref="R100" r:id="rId6" display="Winsource"/>
@@ -27171,7 +27168,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="5"/>
@@ -27231,7 +27228,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44706</v>
+        <v>44728</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -27258,13 +27255,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:26">
       <c r="A5" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>7</v>
@@ -27306,7 +27303,7 @@
         <v>0.1</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>23</v>
@@ -27348,7 +27345,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>23</v>
@@ -27390,7 +27387,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>23</v>
@@ -27432,7 +27429,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>23</v>
@@ -27474,7 +27471,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>23</v>
@@ -27513,10 +27510,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>369</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>370</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>23</v>
@@ -27525,7 +27522,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>26</v>
@@ -27558,7 +27555,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>23</v>
@@ -27600,7 +27597,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>23</v>
@@ -27642,7 +27639,7 @@
         <v>43</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>23</v>
@@ -27682,16 +27679,16 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="E15" s="12" t="s">
         <v>376</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="F15" s="12" t="s">
         <v>377</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>378</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>26</v>
@@ -27722,16 +27719,16 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="E16" s="12" t="s">
         <v>380</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F16" s="12" t="s">
         <v>381</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>382</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>26</v>
@@ -27762,16 +27759,16 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="E17" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>384</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>385</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>26</v>
@@ -27802,7 +27799,7 @@
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>94</v>
@@ -27842,16 +27839,16 @@
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>389</v>
-      </c>
       <c r="F19" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>26</v>
@@ -27882,16 +27879,16 @@
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>392</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>393</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>26</v>
@@ -27922,16 +27919,16 @@
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>396</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>397</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>26</v>
@@ -27962,16 +27959,16 @@
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>400</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>401</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>26</v>
@@ -28002,16 +27999,16 @@
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>404</v>
-      </c>
       <c r="F23" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>26</v>
@@ -28042,16 +28039,16 @@
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>405</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="E24" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="F24" s="12" t="s">
         <v>407</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>408</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>26</v>
@@ -28082,13 +28079,13 @@
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>409</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>410</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>411</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>117</v>
@@ -28122,16 +28119,16 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="E26" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="F26" s="12" t="s">
         <v>414</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>415</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>26</v>
@@ -28162,16 +28159,16 @@
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="E27" s="12" t="s">
         <v>417</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="F27" s="12" t="s">
         <v>418</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>419</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>26</v>
@@ -28202,16 +28199,16 @@
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="E28" s="12" t="s">
         <v>421</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="F28" s="12" t="s">
         <v>422</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>423</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>26</v>
@@ -28242,16 +28239,16 @@
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="E29" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="F29" s="12" t="s">
         <v>426</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>427</v>
       </c>
       <c r="G29" s="18" t="s">
         <v>26</v>
@@ -28282,7 +28279,7 @@
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>125</v>
@@ -28324,7 +28321,7 @@
         <v>120</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>121</v>
@@ -28363,10 +28360,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>430</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>431</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>133</v>
@@ -28375,7 +28372,7 @@
         <v>134</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>26</v>
@@ -28406,16 +28403,16 @@
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="E33" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>434</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>435</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>26</v>
@@ -28448,16 +28445,16 @@
         <v>100</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G34" s="18" t="s">
         <v>26</v>
@@ -28487,19 +28484,19 @@
         <v>13</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G35" s="18" t="s">
         <v>26</v>
@@ -28532,16 +28529,16 @@
         <v>3.01</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>26</v>
@@ -28571,19 +28568,19 @@
         <v>7</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G37" s="18" t="s">
         <v>26</v>
@@ -28613,19 +28610,19 @@
         <v>2</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G38" s="18" t="s">
         <v>26</v>
@@ -28655,19 +28652,19 @@
         <v>1</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G39" s="18" t="s">
         <v>26</v>
@@ -28700,10 +28697,10 @@
         <v>76</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>36</v>
@@ -28739,19 +28736,19 @@
         <v>3</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G41" s="18" t="s">
         <v>26</v>
@@ -28781,19 +28778,19 @@
         <v>1</v>
       </c>
       <c r="B42" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>446</v>
-      </c>
       <c r="D42" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G42" s="18" t="s">
         <v>26</v>
@@ -28823,19 +28820,19 @@
         <v>1</v>
       </c>
       <c r="B43" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>449</v>
-      </c>
       <c r="D43" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G43" s="18" t="s">
         <v>26</v>
@@ -28865,19 +28862,19 @@
         <v>1</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="C44" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>452</v>
-      </c>
       <c r="D44" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>26</v>
@@ -28907,19 +28904,19 @@
         <v>1</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G45" s="18" t="s">
         <v>26</v>
@@ -28949,19 +28946,19 @@
         <v>8</v>
       </c>
       <c r="B46" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="D46" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E46" s="12" t="s">
+      <c r="F46" s="12" t="s">
         <v>457</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>458</v>
       </c>
       <c r="G46" s="18" t="s">
         <v>26</v>
@@ -28992,16 +28989,16 @@
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="E47" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="F47" s="12" t="s">
         <v>461</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>462</v>
       </c>
       <c r="G47" s="18" t="s">
         <v>26</v>
@@ -29032,16 +29029,16 @@
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="E48" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="F48" s="12" t="s">
         <v>465</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>466</v>
       </c>
       <c r="G48" s="18" t="s">
         <v>26</v>
@@ -29072,16 +29069,16 @@
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D49" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="E49" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="F49" s="12" t="s">
         <v>303</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>304</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>26</v>
@@ -29112,16 +29109,16 @@
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="E50" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="F50" s="12" t="s">
         <v>470</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>471</v>
       </c>
       <c r="G50" s="18" t="s">
         <v>26</v>
@@ -29152,16 +29149,16 @@
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="E51" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="F51" s="12" t="s">
         <v>474</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>475</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>26</v>
@@ -29192,16 +29189,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="F52" s="12" t="s">
         <v>478</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>479</v>
       </c>
       <c r="G52" s="18" t="s">
         <v>26</v>
@@ -29232,16 +29229,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="D53" s="12" t="s">
-        <v>481</v>
-      </c>
       <c r="E53" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G53" s="18" t="s">
         <v>26</v>
@@ -29272,16 +29269,16 @@
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G54" s="18" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
received 35 * LTMM-107-02-F-D.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="482">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -1547,13 +1547,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1672,9 +1672,76 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1689,6 +1756,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1696,23 +1778,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1724,10 +1792,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1743,75 +1812,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1899,19 +1899,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1923,31 +1941,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1965,37 +1965,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2013,13 +1989,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2031,43 +2061,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2079,7 +2079,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2499,42 +2499,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2557,6 +2537,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -2564,161 +2564,161 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="30" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2733,7 +2733,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2758,7 +2758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2784,7 +2784,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2883,14 +2883,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2914,7 +2914,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2929,7 +2929,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2953,61 +2953,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3106,16 +3106,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3142,16 +3142,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3421,10 +3421,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D30" activePane="bottomLeft"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="R49" sqref="R49"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D37" workbookViewId="0">
+      <pane ySplit="1170" topLeftCell="D30" activePane="topLeft"/>
+      <selection activeCell="D38" sqref="D38"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3543,7 +3543,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44728</v>
+        <v>44742</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -5179,7 +5179,7 @@
         <v>148.75</v>
       </c>
       <c r="N38" s="106">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="O38" s="106">
         <v>136</v>
@@ -5187,9 +5187,11 @@
       <c r="P38" s="106"/>
       <c r="Q38" s="106">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R38" s="121"/>
+        <v>35</v>
+      </c>
+      <c r="R38" s="121" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="39" customHeight="1" spans="1:18">
       <c r="A39" s="51">
@@ -27228,7 +27230,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44728</v>
+        <v>44742</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
FAN parts arrived to Berkeley.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="486">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -1156,6 +1156,18 @@
     <t>Total:</t>
   </si>
   <si>
+    <t>FAN 92X25MM 24DC LOCK</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 22-24AWG CRIMP GOLD</t>
+  </si>
+  <si>
+    <t>connector, rcpt, 4pos, 2.54mm</t>
+  </si>
+  <si>
+    <t>Newark</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1547,13 +1559,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1673,9 +1685,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1687,10 +1699,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1702,15 +1729,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1726,6 +1761,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1733,30 +1776,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1770,8 +1790,23 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1786,32 +1821,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1899,19 +1911,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1923,7 +1995,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1935,73 +2025,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2013,43 +2037,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2067,13 +2055,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2499,7 +2511,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2515,30 +2542,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2563,162 +2566,171 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="30" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2733,7 +2745,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2784,7 +2796,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2883,14 +2895,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2914,7 +2926,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2929,7 +2941,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2953,7 +2965,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3106,16 +3118,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3421,10 +3433,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D37" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D30" activePane="topLeft"/>
-      <selection activeCell="D38" sqref="D38"/>
-      <selection pane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
+      <pane ySplit="1170" topLeftCell="D105" activePane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="R130" sqref="R130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3543,7 +3555,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44742</v>
+        <v>44823</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -9597,11 +9609,15 @@
     <row r="127" ht="12.75" customHeight="1" spans="1:18">
       <c r="A127" s="144"/>
       <c r="B127" s="145"/>
-      <c r="C127" s="145"/>
+      <c r="C127" s="145" t="s">
+        <v>360</v>
+      </c>
       <c r="D127" s="144"/>
       <c r="E127" s="145"/>
       <c r="F127" s="145"/>
-      <c r="G127" s="156"/>
+      <c r="G127" s="156" t="s">
+        <v>26</v>
+      </c>
       <c r="H127" s="157"/>
       <c r="I127" s="101"/>
       <c r="J127" s="101"/>
@@ -9611,17 +9627,25 @@
       <c r="N127" s="104"/>
       <c r="O127" s="104"/>
       <c r="P127" s="104"/>
-      <c r="Q127" s="104"/>
-      <c r="R127" s="120"/>
+      <c r="Q127" s="104">
+        <v>4</v>
+      </c>
+      <c r="R127" s="120" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="128" ht="12.75" customHeight="1" spans="1:18">
       <c r="A128" s="146"/>
       <c r="B128" s="146"/>
-      <c r="C128" s="146"/>
+      <c r="C128" s="146" t="s">
+        <v>361</v>
+      </c>
       <c r="D128" s="147"/>
       <c r="E128" s="146"/>
       <c r="F128" s="146"/>
-      <c r="G128" s="158"/>
+      <c r="G128" s="158" t="s">
+        <v>26</v>
+      </c>
       <c r="H128" s="159"/>
       <c r="I128" s="103"/>
       <c r="J128" s="103"/>
@@ -9631,17 +9655,25 @@
       <c r="N128" s="104"/>
       <c r="O128" s="104"/>
       <c r="P128" s="104"/>
-      <c r="Q128" s="104"/>
-      <c r="R128" s="120"/>
+      <c r="Q128" s="104">
+        <v>100</v>
+      </c>
+      <c r="R128" s="120" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="129" ht="12.75" customHeight="1" spans="1:18">
       <c r="A129" s="146"/>
       <c r="B129" s="146"/>
-      <c r="C129" s="146"/>
+      <c r="C129" s="146" t="s">
+        <v>362</v>
+      </c>
       <c r="D129" s="147"/>
       <c r="E129" s="146"/>
       <c r="F129" s="146"/>
-      <c r="G129" s="158"/>
+      <c r="G129" s="158" t="s">
+        <v>363</v>
+      </c>
       <c r="H129" s="159"/>
       <c r="I129" s="103"/>
       <c r="J129" s="103"/>
@@ -9651,8 +9683,12 @@
       <c r="N129" s="104"/>
       <c r="O129" s="104"/>
       <c r="P129" s="104"/>
-      <c r="Q129" s="104"/>
-      <c r="R129" s="120"/>
+      <c r="Q129" s="104">
+        <v>100</v>
+      </c>
+      <c r="R129" s="120" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="130" ht="12.75" customHeight="1" spans="1:18">
       <c r="A130" s="146"/>
@@ -27170,7 +27206,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="14" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="5"/>
@@ -27230,7 +27266,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44742</v>
+        <v>44823</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -27257,13 +27293,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:26">
       <c r="A5" s="8" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>7</v>
@@ -27305,7 +27341,7 @@
         <v>0.1</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>23</v>
@@ -27347,7 +27383,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>23</v>
@@ -27389,7 +27425,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>23</v>
@@ -27431,7 +27467,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>23</v>
@@ -27473,7 +27509,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>23</v>
@@ -27512,10 +27548,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>23</v>
@@ -27524,7 +27560,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>26</v>
@@ -27557,7 +27593,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>23</v>
@@ -27599,7 +27635,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>23</v>
@@ -27641,7 +27677,7 @@
         <v>43</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>23</v>
@@ -27681,16 +27717,16 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>26</v>
@@ -27721,16 +27757,16 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>26</v>
@@ -27761,16 +27797,16 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>26</v>
@@ -27801,7 +27837,7 @@
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>94</v>
@@ -27841,16 +27877,16 @@
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>26</v>
@@ -27881,16 +27917,16 @@
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>26</v>
@@ -27921,16 +27957,16 @@
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>26</v>
@@ -27961,16 +27997,16 @@
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>26</v>
@@ -28001,16 +28037,16 @@
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>26</v>
@@ -28041,16 +28077,16 @@
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>26</v>
@@ -28081,13 +28117,13 @@
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>117</v>
@@ -28121,16 +28157,16 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>26</v>
@@ -28161,16 +28197,16 @@
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>26</v>
@@ -28201,16 +28237,16 @@
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>26</v>
@@ -28241,16 +28277,16 @@
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="G29" s="18" t="s">
         <v>26</v>
@@ -28281,7 +28317,7 @@
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>125</v>
@@ -28323,7 +28359,7 @@
         <v>120</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>121</v>
@@ -28362,10 +28398,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>133</v>
@@ -28374,7 +28410,7 @@
         <v>134</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>26</v>
@@ -28405,16 +28441,16 @@
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>26</v>
@@ -28447,7 +28483,7 @@
         <v>100</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>163</v>
@@ -28489,7 +28525,7 @@
         <v>177</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>163</v>
@@ -28531,7 +28567,7 @@
         <v>3.01</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>163</v>
@@ -28540,7 +28576,7 @@
         <v>36</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>26</v>
@@ -28573,7 +28609,7 @@
         <v>204</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>163</v>
@@ -28615,7 +28651,7 @@
         <v>173</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>163</v>
@@ -28657,7 +28693,7 @@
         <v>198</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>163</v>
@@ -28699,7 +28735,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>163</v>
@@ -28741,7 +28777,7 @@
         <v>196</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>163</v>
@@ -28780,10 +28816,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>163</v>
@@ -28792,7 +28828,7 @@
         <v>36</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="G42" s="18" t="s">
         <v>26</v>
@@ -28822,10 +28858,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>163</v>
@@ -28834,7 +28870,7 @@
         <v>36</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="G43" s="18" t="s">
         <v>26</v>
@@ -28864,10 +28900,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>163</v>
@@ -28876,7 +28912,7 @@
         <v>36</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>26</v>
@@ -28909,7 +28945,7 @@
         <v>236</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>163</v>
@@ -28948,19 +28984,19 @@
         <v>8</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>163</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="G46" s="18" t="s">
         <v>26</v>
@@ -28991,16 +29027,16 @@
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="G47" s="18" t="s">
         <v>26</v>
@@ -29031,16 +29067,16 @@
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="G48" s="18" t="s">
         <v>26</v>
@@ -29071,7 +29107,7 @@
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>301</v>
@@ -29111,16 +29147,16 @@
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="G50" s="18" t="s">
         <v>26</v>
@@ -29151,16 +29187,16 @@
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>26</v>
@@ -29191,16 +29227,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="G52" s="18" t="s">
         <v>26</v>
@@ -29231,16 +29267,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="E53" s="12" t="s">
         <v>297</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="G53" s="18" t="s">
         <v>26</v>
@@ -29271,7 +29307,7 @@
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>322</v>

</xml_diff>

<commit_message>
updated the number of maroc chips.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="12525"/>
+    <workbookView windowWidth="28800" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="quabo" sheetId="1" r:id="rId1"/>
@@ -806,7 +806,7 @@
     <t>Weeroc</t>
   </si>
   <si>
-    <t>1*QFP + 19*BGA</t>
+    <t>2*QFP + 19*BGA</t>
   </si>
   <si>
     <t>XC7K160T-1FFG676C</t>
@@ -1559,13 +1559,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="180" formatCode="[$-C09]dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1692,32 +1692,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1729,14 +1707,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1745,7 +1715,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1754,14 +1724,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1783,7 +1745,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1797,6 +1781,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1805,8 +1804,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1814,14 +1822,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1911,31 +1911,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1953,13 +1959,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1971,127 +2091,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2492,21 +2492,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2531,6 +2516,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2542,6 +2536,36 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2565,169 +2589,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="16" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2745,7 +2745,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2770,7 +2770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2796,7 +2796,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2895,14 +2895,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2926,7 +2926,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2941,7 +2941,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2965,61 +2965,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3118,16 +3118,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3154,16 +3154,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3434,9 +3434,9 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D105" activePane="bottomLeft"/>
+      <pane ySplit="1170" topLeftCell="D84" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R130" sqref="R130"/>
+      <selection pane="bottomLeft" activeCell="R93" sqref="R93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3555,7 +3555,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44823</v>
+        <v>44852</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -7913,11 +7913,11 @@
         <v>0</v>
       </c>
       <c r="P93" s="104">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q93" s="104">
         <f t="shared" si="15"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R93" s="120" t="s">
         <v>249</v>
@@ -27266,7 +27266,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44823</v>
+        <v>44852</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
received: 10 * MMBT3906T-TP; 10 * ADCMP605BCPZ-R7; 50 * OPA2376AIDR; 24 * TMP125AIDBVR; 05 * LT1965IT#PBF; 16 * LT1965EMS8E#PBF; 10 * S25FL256LAGNFV010.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="488">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -533,405 +533,408 @@
     <t>MMBT3906TCT-ND</t>
   </si>
   <si>
+    <t>Rochester, RAL Dig Lab. They are from digi-key</t>
+  </si>
+  <si>
+    <t>LND150</t>
+  </si>
+  <si>
+    <t>LND150K1-GCT-ND</t>
+  </si>
+  <si>
+    <t>Expected 12/19/22</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Res</t>
+  </si>
+  <si>
+    <t>P100HCT</t>
+  </si>
+  <si>
+    <t>3/15/2022</t>
+  </si>
+  <si>
+    <t>5mohm/1W</t>
+  </si>
+  <si>
+    <t>0805wide</t>
+  </si>
+  <si>
+    <t>408-1595-1-ND</t>
+  </si>
+  <si>
+    <t>150k</t>
+  </si>
+  <si>
+    <t>P150KHCT</t>
+  </si>
+  <si>
+    <t>6.65k</t>
+  </si>
+  <si>
+    <t>P6.65KHCT</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>P0.0GCT</t>
+  </si>
+  <si>
+    <t>4.99K</t>
+  </si>
+  <si>
+    <t>P4.99KHCT</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>P10.0KHCT</t>
+  </si>
+  <si>
+    <t>1.10k</t>
+  </si>
+  <si>
+    <t>P1.10KHCT</t>
+  </si>
+  <si>
+    <t>301k 0.1%</t>
+  </si>
+  <si>
+    <t>P301KDBCT</t>
+  </si>
+  <si>
+    <t>249</t>
+  </si>
+  <si>
+    <t>P249HCT</t>
+  </si>
+  <si>
+    <t>7.87k 0.1%</t>
+  </si>
+  <si>
+    <t>YAG1736CT</t>
+  </si>
+  <si>
+    <t>7.5k</t>
+  </si>
+  <si>
+    <t>P7.50KHCT</t>
+  </si>
+  <si>
+    <t>4.99k 0.1%</t>
+  </si>
+  <si>
+    <t>P4.99KDBCT</t>
+  </si>
+  <si>
+    <t>499</t>
+  </si>
+  <si>
+    <t>P499HCT</t>
+  </si>
+  <si>
+    <t>499k 0.1%</t>
+  </si>
+  <si>
+    <t>YAG4565CT</t>
+  </si>
+  <si>
+    <t>6/29/2022</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>541-100KSCT-ND</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>311-1.00MHRCT-ND</t>
+  </si>
+  <si>
+    <t>27.4k</t>
+  </si>
+  <si>
+    <t>P27.4KHCT</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>P237HCT</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>P1.00KHCT</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>P4.70KHCT</t>
+  </si>
+  <si>
+    <t>2.4k</t>
+  </si>
+  <si>
+    <t>P2.40KHCT</t>
+  </si>
+  <si>
+    <t>49.9</t>
+  </si>
+  <si>
+    <t>P49.9HCT</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>P15.0HCT</t>
+  </si>
+  <si>
+    <t>1/18/2022 ?</t>
+  </si>
+  <si>
+    <t>63.4k</t>
+  </si>
+  <si>
+    <t>P63.4KHCT</t>
+  </si>
+  <si>
+    <t>10k 0.1%</t>
+  </si>
+  <si>
+    <t>P10KDBCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	7/25/2022</t>
+  </si>
+  <si>
+    <t>383k</t>
+  </si>
+  <si>
+    <t>P383KHCT</t>
+  </si>
+  <si>
+    <t>1.74k</t>
+  </si>
+  <si>
+    <t>P1.74KHCT</t>
+  </si>
+  <si>
+    <t>18.2k</t>
+  </si>
+  <si>
+    <t>P18.2KHCT</t>
+  </si>
+  <si>
+    <t>140k</t>
+  </si>
+  <si>
+    <t>P140KHCT</t>
+  </si>
+  <si>
+    <t>442</t>
+  </si>
+  <si>
+    <t>P442HCT</t>
+  </si>
+  <si>
+    <t>732</t>
+  </si>
+  <si>
+    <t>P732HCT</t>
+  </si>
+  <si>
+    <t>604</t>
+  </si>
+  <si>
+    <t>P604HCT</t>
+  </si>
+  <si>
+    <t>3.32k</t>
+  </si>
+  <si>
+    <t>P3.32KHCT</t>
+  </si>
+  <si>
+    <t>40.2k</t>
+  </si>
+  <si>
+    <t>P40.2KHCT</t>
+  </si>
+  <si>
+    <t>806</t>
+  </si>
+  <si>
+    <t>P806HCT</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>P200HCT</t>
+  </si>
+  <si>
+    <t>res_0201</t>
+  </si>
+  <si>
+    <t>541-49.9ABCT</t>
+  </si>
+  <si>
+    <t>through-hole pad</t>
+  </si>
+  <si>
+    <t>TP_EX_SMALL</t>
+  </si>
+  <si>
+    <t>MAROC3A_BGA</t>
+  </si>
+  <si>
+    <t>Maroc_BGA353_.5mm</t>
+  </si>
+  <si>
+    <t>Weeroc</t>
+  </si>
+  <si>
+    <t>2*QFP + 19*BGA</t>
+  </si>
+  <si>
+    <t>XC7K160T-1FFG676C</t>
+  </si>
+  <si>
+    <t>FFG676</t>
+  </si>
+  <si>
+    <t>122-2098-ND</t>
+  </si>
+  <si>
+    <t>4/20/2022</t>
+  </si>
+  <si>
+    <t>LTC6090IS8E</t>
+  </si>
+  <si>
+    <t>SO8_LT6090</t>
+  </si>
+  <si>
+    <t>LTC6090CS8E#PBF-ND</t>
+  </si>
+  <si>
+    <t>3/16/2022</t>
+  </si>
+  <si>
+    <t>OPA2376AIDR</t>
+  </si>
+  <si>
+    <t>TI-D8_N</t>
+  </si>
+  <si>
+    <t>296-22564-1-ND</t>
+  </si>
+  <si>
+    <t>Winsource, RAL Dig Lab</t>
+  </si>
+  <si>
+    <t>74AVC2T245</t>
+  </si>
+  <si>
+    <t>QFP10_NL</t>
+  </si>
+  <si>
+    <t>296-23684-1-ND</t>
+  </si>
+  <si>
+    <t>S25FL256_8WSON</t>
+  </si>
+  <si>
+    <t>WSON-8_6x8mm</t>
+  </si>
+  <si>
+    <t>428-4096-ND</t>
+  </si>
+  <si>
+    <t>LTC3611IWP</t>
+  </si>
+  <si>
+    <t>QFN64_LTC3611</t>
+  </si>
+  <si>
+    <t>LTC3611IWP#PBF-ND</t>
+  </si>
+  <si>
+    <t>1/17/2022 ?</t>
+  </si>
+  <si>
+    <t>INA333</t>
+  </si>
+  <si>
+    <t>msop-ua8_l</t>
+  </si>
+  <si>
+    <t>296-23564-1-ND</t>
+  </si>
+  <si>
+    <t>Winsource</t>
+  </si>
+  <si>
+    <t>LP5951MF-3.0/NOPB</t>
+  </si>
+  <si>
+    <t>MF05A_N</t>
+  </si>
+  <si>
+    <t>LP5951MF-3.0/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>VM53S3</t>
+  </si>
+  <si>
+    <t>VM53S3-25.000-2.5/-30+85</t>
+  </si>
+  <si>
+    <t>Dove</t>
+  </si>
+  <si>
+    <t>Dan have some. we also received 7 from Linclon.</t>
+  </si>
+  <si>
+    <t>CDCM61004RHB</t>
+  </si>
+  <si>
+    <t>QFN32</t>
+  </si>
+  <si>
+    <t>296-24194-1-ND</t>
+  </si>
+  <si>
+    <t>9/22/2022</t>
+  </si>
+  <si>
+    <t>AD5662BRJ-1REEL7</t>
+  </si>
+  <si>
+    <t>RJ-8_N</t>
+  </si>
+  <si>
+    <t>AD5662BRJZ-1REEL7CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	8/17/2022</t>
+  </si>
+  <si>
     <t>Rochester</t>
   </si>
   <si>
-    <t>LND150</t>
-  </si>
-  <si>
-    <t>LND150K1-GCT-ND</t>
-  </si>
-  <si>
-    <t>Expected 12/19/22</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Res</t>
-  </si>
-  <si>
-    <t>P100HCT</t>
-  </si>
-  <si>
-    <t>3/15/2022</t>
-  </si>
-  <si>
-    <t>5mohm/1W</t>
-  </si>
-  <si>
-    <t>0805wide</t>
-  </si>
-  <si>
-    <t>408-1595-1-ND</t>
-  </si>
-  <si>
-    <t>150k</t>
-  </si>
-  <si>
-    <t>P150KHCT</t>
-  </si>
-  <si>
-    <t>6.65k</t>
-  </si>
-  <si>
-    <t>P6.65KHCT</t>
-  </si>
-  <si>
-    <t>zero</t>
-  </si>
-  <si>
-    <t>P0.0GCT</t>
-  </si>
-  <si>
-    <t>4.99K</t>
-  </si>
-  <si>
-    <t>P4.99KHCT</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>P10.0KHCT</t>
-  </si>
-  <si>
-    <t>1.10k</t>
-  </si>
-  <si>
-    <t>P1.10KHCT</t>
-  </si>
-  <si>
-    <t>301k 0.1%</t>
-  </si>
-  <si>
-    <t>P301KDBCT</t>
-  </si>
-  <si>
-    <t>249</t>
-  </si>
-  <si>
-    <t>P249HCT</t>
-  </si>
-  <si>
-    <t>7.87k 0.1%</t>
-  </si>
-  <si>
-    <t>YAG1736CT</t>
-  </si>
-  <si>
-    <t>7.5k</t>
-  </si>
-  <si>
-    <t>P7.50KHCT</t>
-  </si>
-  <si>
-    <t>4.99k 0.1%</t>
-  </si>
-  <si>
-    <t>P4.99KDBCT</t>
-  </si>
-  <si>
-    <t>499</t>
-  </si>
-  <si>
-    <t>P499HCT</t>
-  </si>
-  <si>
-    <t>499k 0.1%</t>
-  </si>
-  <si>
-    <t>YAG4565CT</t>
-  </si>
-  <si>
-    <t>6/29/2022</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>541-100KSCT-ND</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>311-1.00MHRCT-ND</t>
-  </si>
-  <si>
-    <t>27.4k</t>
-  </si>
-  <si>
-    <t>P27.4KHCT</t>
-  </si>
-  <si>
-    <t>237</t>
-  </si>
-  <si>
-    <t>P237HCT</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>P1.00KHCT</t>
-  </si>
-  <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>P4.70KHCT</t>
-  </si>
-  <si>
-    <t>2.4k</t>
-  </si>
-  <si>
-    <t>P2.40KHCT</t>
-  </si>
-  <si>
-    <t>49.9</t>
-  </si>
-  <si>
-    <t>P49.9HCT</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>P15.0HCT</t>
-  </si>
-  <si>
-    <t>1/18/2022 ?</t>
-  </si>
-  <si>
-    <t>63.4k</t>
-  </si>
-  <si>
-    <t>P63.4KHCT</t>
-  </si>
-  <si>
-    <t>10k 0.1%</t>
-  </si>
-  <si>
-    <t>P10KDBCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	7/25/2022</t>
-  </si>
-  <si>
-    <t>383k</t>
-  </si>
-  <si>
-    <t>P383KHCT</t>
-  </si>
-  <si>
-    <t>1.74k</t>
-  </si>
-  <si>
-    <t>P1.74KHCT</t>
-  </si>
-  <si>
-    <t>18.2k</t>
-  </si>
-  <si>
-    <t>P18.2KHCT</t>
-  </si>
-  <si>
-    <t>140k</t>
-  </si>
-  <si>
-    <t>P140KHCT</t>
-  </si>
-  <si>
-    <t>442</t>
-  </si>
-  <si>
-    <t>P442HCT</t>
-  </si>
-  <si>
-    <t>732</t>
-  </si>
-  <si>
-    <t>P732HCT</t>
-  </si>
-  <si>
-    <t>604</t>
-  </si>
-  <si>
-    <t>P604HCT</t>
-  </si>
-  <si>
-    <t>3.32k</t>
-  </si>
-  <si>
-    <t>P3.32KHCT</t>
-  </si>
-  <si>
-    <t>40.2k</t>
-  </si>
-  <si>
-    <t>P40.2KHCT</t>
-  </si>
-  <si>
-    <t>806</t>
-  </si>
-  <si>
-    <t>P806HCT</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>P200HCT</t>
-  </si>
-  <si>
-    <t>res_0201</t>
-  </si>
-  <si>
-    <t>541-49.9ABCT</t>
-  </si>
-  <si>
-    <t>through-hole pad</t>
-  </si>
-  <si>
-    <t>TP_EX_SMALL</t>
-  </si>
-  <si>
-    <t>MAROC3A_BGA</t>
-  </si>
-  <si>
-    <t>Maroc_BGA353_.5mm</t>
-  </si>
-  <si>
-    <t>Weeroc</t>
-  </si>
-  <si>
-    <t>2*QFP + 19*BGA</t>
-  </si>
-  <si>
-    <t>XC7K160T-1FFG676C</t>
-  </si>
-  <si>
-    <t>FFG676</t>
-  </si>
-  <si>
-    <t>122-2098-ND</t>
-  </si>
-  <si>
-    <t>4/20/2022</t>
-  </si>
-  <si>
-    <t>LTC6090IS8E</t>
-  </si>
-  <si>
-    <t>SO8_LT6090</t>
-  </si>
-  <si>
-    <t>LTC6090CS8E#PBF-ND</t>
-  </si>
-  <si>
-    <t>3/16/2022</t>
-  </si>
-  <si>
-    <t>OPA2376AIDR</t>
-  </si>
-  <si>
-    <t>TI-D8_N</t>
-  </si>
-  <si>
-    <t>296-22564-1-ND</t>
-  </si>
-  <si>
-    <t>Winsource</t>
-  </si>
-  <si>
-    <t>74AVC2T245</t>
-  </si>
-  <si>
-    <t>QFP10_NL</t>
-  </si>
-  <si>
-    <t>296-23684-1-ND</t>
-  </si>
-  <si>
-    <t>S25FL256_8WSON</t>
-  </si>
-  <si>
-    <t>WSON-8_6x8mm</t>
-  </si>
-  <si>
-    <t>428-4096-ND</t>
-  </si>
-  <si>
-    <t>expected 11/25/22</t>
-  </si>
-  <si>
-    <t>LTC3611IWP</t>
-  </si>
-  <si>
-    <t>QFN64_LTC3611</t>
-  </si>
-  <si>
-    <t>LTC3611IWP#PBF-ND</t>
-  </si>
-  <si>
-    <t>1/17/2022 ?</t>
-  </si>
-  <si>
-    <t>INA333</t>
-  </si>
-  <si>
-    <t>msop-ua8_l</t>
-  </si>
-  <si>
-    <t>296-23564-1-ND</t>
-  </si>
-  <si>
-    <t>LP5951MF-3.0/NOPB</t>
-  </si>
-  <si>
-    <t>MF05A_N</t>
-  </si>
-  <si>
-    <t>LP5951MF-3.0/NOPBCT-ND</t>
-  </si>
-  <si>
-    <t>VM53S3</t>
-  </si>
-  <si>
-    <t>VM53S3-25.000-2.5/-30+85</t>
-  </si>
-  <si>
-    <t>Dove</t>
-  </si>
-  <si>
-    <t>Dan have some. we also received 7 from Linclon.</t>
-  </si>
-  <si>
-    <t>CDCM61004RHB</t>
-  </si>
-  <si>
-    <t>QFN32</t>
-  </si>
-  <si>
-    <t>296-24194-1-ND</t>
-  </si>
-  <si>
-    <t>9/22/2022</t>
-  </si>
-  <si>
-    <t>AD5662BRJ-1REEL7</t>
-  </si>
-  <si>
-    <t>RJ-8_N</t>
-  </si>
-  <si>
-    <t>AD5662BRJZ-1REEL7CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	8/17/2022</t>
-  </si>
-  <si>
     <t>CDCM61004RHB_DNP</t>
   </si>
   <si>
@@ -959,7 +962,7 @@
     <t>1/24/2023</t>
   </si>
   <si>
-    <t>5*LT1965EMS8E#PBF + 9*LT1965IMS8E-1.8#PBF</t>
+    <t>9*LT1965IMS8E-1.8#PBF</t>
   </si>
   <si>
     <t>LT8609S</t>
@@ -1022,7 +1025,7 @@
     <t>296-28002-1-ND</t>
   </si>
   <si>
-    <t>ztz technology</t>
+    <t>ztz technology, RAL Dig Lab</t>
   </si>
   <si>
     <t>LT1965EMS8E-3.3#PBF</t>
@@ -1081,6 +1084,9 @@
     <t>LT1965EMS8E#TRPBF-ND</t>
   </si>
   <si>
+    <t>RAL Dig Lab, 5*LT1965EMS8E#PBF  + 5*LT1965IT#PBF +16*LT1965EMS8E#PBF</t>
+  </si>
+  <si>
     <t>ADR441ARZ</t>
   </si>
   <si>
@@ -1123,7 +1129,7 @@
     <t>ADCMP605BCPZ-R2-ND</t>
   </si>
   <si>
-    <t>Mouser</t>
+    <t>Mouser,RAL Dig Lab, ADCMP605BCPZ-R7</t>
   </si>
   <si>
     <t>20 MHz VCXO CMOS Oscillator 3.3V Enable/Disable 6-SMD, No Lead</t>
@@ -1559,13 +1565,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-C09]dd\-mmm\-yy"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1684,6 +1690,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1692,25 +1736,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1722,16 +1751,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1746,38 +1775,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1798,23 +1804,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1917,7 +1923,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1929,19 +2055,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1953,139 +2085,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2507,6 +2513,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2539,44 +2578,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2592,145 +2598,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="37" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2745,7 +2751,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2770,7 +2776,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2796,7 +2802,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2895,14 +2901,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2926,7 +2932,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2941,7 +2947,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2965,61 +2971,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3118,16 +3124,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3154,16 +3160,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3433,10 +3439,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D90" activePane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
+      <pane ySplit="1170" topLeftCell="D87" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D109" sqref="$A109:$XFD109"/>
+      <selection pane="bottomLeft" activeCell="R113" sqref="R113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3555,7 +3561,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44852</v>
+        <v>44944</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -5885,14 +5891,16 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N51" s="114"/>
+      <c r="N51" s="114">
+        <v>10</v>
+      </c>
       <c r="O51" s="114" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="P51" s="114"/>
       <c r="Q51" s="114">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R51" s="127" t="s">
         <v>158</v>
@@ -8067,7 +8075,9 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N96" s="114"/>
+      <c r="N96" s="114">
+        <v>50</v>
+      </c>
       <c r="O96" s="114">
         <v>829.44</v>
       </c>
@@ -8076,7 +8086,7 @@
       </c>
       <c r="Q96" s="114">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="R96" s="127" t="s">
         <v>261</v>
@@ -8177,7 +8187,9 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N98" s="161"/>
+      <c r="N98" s="161">
+        <v>10</v>
+      </c>
       <c r="O98" s="161">
         <v>193.28</v>
       </c>
@@ -8186,10 +8198,10 @@
       </c>
       <c r="Q98" s="161">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="R98" s="165" t="s">
-        <v>268</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" ht="14" customHeight="1" spans="1:18">
@@ -8201,19 +8213,19 @@
       </c>
       <c r="C99" s="136"/>
       <c r="D99" s="137" t="s">
+        <v>268</v>
+      </c>
+      <c r="E99" s="137" t="s">
         <v>269</v>
       </c>
-      <c r="E99" s="137" t="s">
+      <c r="F99" s="137" t="s">
         <v>270</v>
-      </c>
-      <c r="F99" s="137" t="s">
-        <v>271</v>
       </c>
       <c r="G99" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H99" s="91" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I99" s="109">
         <v>24.18</v>
@@ -8250,13 +8262,13 @@
       </c>
       <c r="C100" s="132"/>
       <c r="D100" s="132" t="s">
+        <v>272</v>
+      </c>
+      <c r="E100" s="132" t="s">
         <v>273</v>
       </c>
-      <c r="E100" s="132" t="s">
+      <c r="F100" s="132" t="s">
         <v>274</v>
-      </c>
-      <c r="F100" s="132" t="s">
-        <v>275</v>
       </c>
       <c r="G100" s="94" t="s">
         <v>26</v>
@@ -8291,7 +8303,7 @@
         <v>1</v>
       </c>
       <c r="R100" s="127" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="101" ht="14" customHeight="1" spans="1:18">
@@ -8454,7 +8466,7 @@
         <v>10</v>
       </c>
       <c r="R103" s="127" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
     </row>
     <row r="104" ht="13" customHeight="1" spans="1:18">
@@ -8507,7 +8519,7 @@
         <v>1</v>
       </c>
       <c r="R104" s="127" t="s">
-        <v>158</v>
+        <v>291</v>
       </c>
     </row>
     <row r="105" ht="13" customHeight="1" spans="1:18">
@@ -8519,7 +8531,7 @@
       </c>
       <c r="C105" s="60"/>
       <c r="D105" s="61" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E105" s="61" t="s">
         <v>284</v>
@@ -8558,7 +8570,7 @@
         <v>0</v>
       </c>
       <c r="R105" s="127" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="106" ht="12" customHeight="1" spans="1:18">
@@ -8570,13 +8582,13 @@
       </c>
       <c r="C106" s="55"/>
       <c r="D106" s="55" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E106" s="55" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F106" s="55" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G106" s="90" t="s">
         <v>26</v>
@@ -8619,19 +8631,19 @@
       </c>
       <c r="C107" s="49"/>
       <c r="D107" s="50" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E107" s="50" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F107" s="50" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G107" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H107" s="88" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I107" s="107">
         <v>6.71</v>
@@ -8653,14 +8665,14 @@
         <v>858.88</v>
       </c>
       <c r="P107" s="108">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="Q107" s="108">
         <f t="shared" si="15"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="R107" s="122" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="108" ht="12.75" customHeight="1" spans="1:18">
@@ -8672,19 +8684,19 @@
       </c>
       <c r="C108" s="55"/>
       <c r="D108" s="55" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E108" s="55" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F108" s="55" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G108" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H108" s="91" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="I108" s="109">
         <v>7.97</v>
@@ -8713,7 +8725,7 @@
         <v>8</v>
       </c>
       <c r="R108" s="123" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="109" ht="12.75" customHeight="1" spans="1:18">
@@ -8725,19 +8737,19 @@
       </c>
       <c r="C109" s="52"/>
       <c r="D109" s="53" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E109" s="53" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F109" s="53" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G109" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H109" s="86" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I109" s="105">
         <v>5.14</v>
@@ -8780,19 +8792,19 @@
       </c>
       <c r="C110" s="47"/>
       <c r="D110" s="47" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E110" s="47" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F110" s="47" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G110" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H110" s="86" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I110" s="105">
         <v>51.06</v>
@@ -8835,13 +8847,13 @@
       </c>
       <c r="C111" s="52"/>
       <c r="D111" s="53" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E111" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="F111" s="53" t="s">
         <v>315</v>
-      </c>
-      <c r="F111" s="53" t="s">
-        <v>314</v>
       </c>
       <c r="G111" s="85" t="s">
         <v>26</v>
@@ -8892,13 +8904,13 @@
       </c>
       <c r="C112" s="47"/>
       <c r="D112" s="47" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E112" s="47" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F112" s="47" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G112" s="85" t="s">
         <v>26</v>
@@ -8947,13 +8959,13 @@
       </c>
       <c r="C113" s="60"/>
       <c r="D113" s="61" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E113" s="61" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F113" s="61" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G113" s="94" t="s">
         <v>26</v>
@@ -8976,7 +8988,9 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N113" s="114"/>
+      <c r="N113" s="114">
+        <v>24</v>
+      </c>
       <c r="O113" s="114">
         <v>104.32</v>
       </c>
@@ -8985,10 +8999,10 @@
       </c>
       <c r="Q113" s="114">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="R113" s="127" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="114" ht="13" customHeight="1" spans="1:18">
@@ -9000,19 +9014,19 @@
       </c>
       <c r="C114" s="130"/>
       <c r="D114" s="130" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E114" s="130" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F114" s="130" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G114" s="87" t="s">
         <v>26</v>
       </c>
       <c r="H114" s="88" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I114" s="107">
         <v>5.87</v>
@@ -9049,13 +9063,13 @@
       </c>
       <c r="C115" s="60"/>
       <c r="D115" s="61" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E115" s="61" t="s">
         <v>145</v>
       </c>
       <c r="F115" s="61" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G115" s="94" t="s">
         <v>26</v>
@@ -9090,7 +9104,7 @@
         <v>2</v>
       </c>
       <c r="R115" s="125" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="116" ht="12" customHeight="1" spans="1:18">
@@ -9102,10 +9116,10 @@
       </c>
       <c r="C116" s="47"/>
       <c r="D116" s="47" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E116" s="47" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F116" s="47" t="s">
         <v>76</v>
@@ -9149,13 +9163,13 @@
       </c>
       <c r="C117" s="60"/>
       <c r="D117" s="61" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E117" s="61" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F117" s="61" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G117" s="94" t="s">
         <v>26</v>
@@ -9188,7 +9202,7 @@
         <v>0</v>
       </c>
       <c r="R117" s="127" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="118" ht="13" customHeight="1" spans="1:18">
@@ -9200,19 +9214,19 @@
       </c>
       <c r="C118" s="55"/>
       <c r="D118" s="55" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E118" s="55" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F118" s="55" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="G118" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H118" s="91" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I118" s="109">
         <v>5.87</v>
@@ -9229,16 +9243,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N118" s="110"/>
+      <c r="N118" s="110">
+        <v>26</v>
+      </c>
       <c r="O118" s="110">
         <v>375.68</v>
       </c>
       <c r="P118" s="110"/>
       <c r="Q118" s="110">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R118" s="123"/>
+        <v>26</v>
+      </c>
+      <c r="R118" s="123" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="119" ht="12.75" customHeight="1" spans="1:18">
       <c r="A119" s="51">
@@ -9249,19 +9267,19 @@
       </c>
       <c r="C119" s="52"/>
       <c r="D119" s="53" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="E119" s="53" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F119" s="53" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="G119" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H119" s="86" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="I119" s="105">
         <v>7.34</v>
@@ -9306,19 +9324,19 @@
       </c>
       <c r="C120" s="47"/>
       <c r="D120" s="47" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E120" s="47" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="F120" s="47" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="G120" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H120" s="86" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="I120" s="105">
         <v>4.94</v>
@@ -9363,19 +9381,19 @@
       </c>
       <c r="C121" s="52"/>
       <c r="D121" s="53" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E121" s="53" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="F121" s="53" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="G121" s="85" t="s">
         <v>26</v>
       </c>
       <c r="H121" s="86" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="I121" s="105">
         <v>9.64</v>
@@ -9418,13 +9436,13 @@
       </c>
       <c r="C122" s="132"/>
       <c r="D122" s="132" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E122" s="132" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="F122" s="132" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="G122" s="94" t="s">
         <v>127</v>
@@ -9445,17 +9463,19 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N122" s="114"/>
+      <c r="N122" s="114">
+        <v>10</v>
+      </c>
       <c r="O122" s="114">
         <v>0</v>
       </c>
       <c r="P122" s="114"/>
       <c r="Q122" s="114">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R122" s="127" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="123" ht="12.75" customHeight="1" spans="1:18">
@@ -9466,16 +9486,16 @@
         <v>38</v>
       </c>
       <c r="C123" s="57" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D123" s="58" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E123" s="58" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F123" s="58" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G123" s="92" t="s">
         <v>127</v>
@@ -9518,19 +9538,19 @@
       </c>
       <c r="C124" s="139"/>
       <c r="D124" s="139" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E124" s="139" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="F124" s="139" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G124" s="152" t="s">
         <v>26</v>
       </c>
       <c r="H124" s="91" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="I124" s="109">
         <v>5.83</v>
@@ -9559,7 +9579,7 @@
         <v>2</v>
       </c>
       <c r="R124" s="123" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="125" ht="28" customHeight="1" spans="1:18">
@@ -9572,7 +9592,7 @@
       <c r="G125" s="153"/>
       <c r="H125" s="154"/>
       <c r="I125" s="162" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="J125" s="163">
         <f>SUM(J6:J124)</f>
@@ -9614,7 +9634,7 @@
       <c r="A127" s="144"/>
       <c r="B127" s="145"/>
       <c r="C127" s="145" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D127" s="144"/>
       <c r="E127" s="145"/>
@@ -9642,7 +9662,7 @@
       <c r="A128" s="146"/>
       <c r="B128" s="146"/>
       <c r="C128" s="146" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D128" s="147"/>
       <c r="E128" s="146"/>
@@ -9670,13 +9690,13 @@
       <c r="A129" s="146"/>
       <c r="B129" s="146"/>
       <c r="C129" s="146" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D129" s="147"/>
       <c r="E129" s="146"/>
       <c r="F129" s="146"/>
       <c r="G129" s="158" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="H129" s="159"/>
       <c r="I129" s="103"/>
@@ -27142,16 +27162,16 @@
     <hyperlink ref="E2" r:id="rId1" display="Quabo_BGA.PrjPcb&#10;From:17.08.DN001.v06_Quabo_BOM"/>
     <hyperlink ref="R47" r:id="rId2" display="From Mouser"/>
     <hyperlink ref="R49" r:id="rId3" display="RAL Dig Lab"/>
-    <hyperlink ref="R51" r:id="rId4" display="Rochester"/>
-    <hyperlink ref="R96" r:id="rId5" display="Winsource"/>
+    <hyperlink ref="R51" r:id="rId4" display="Rochester, RAL Dig Lab. They are from digi-key"/>
+    <hyperlink ref="R96" r:id="rId5" display="Winsource, RAL Dig Lab"/>
     <hyperlink ref="R100" r:id="rId6" display="Winsource"/>
     <hyperlink ref="R103" r:id="rId7" display="Winsource"/>
     <hyperlink ref="R104" r:id="rId8" display="Rochester"/>
     <hyperlink ref="R105" r:id="rId7" display="WinSource"/>
-    <hyperlink ref="R113" r:id="rId9" display="ztz technology"/>
+    <hyperlink ref="R113" r:id="rId9" display="ztz technology, RAL Dig Lab"/>
     <hyperlink ref="R115" r:id="rId10" display="Winsource ? Not sure, no PBCT-ND"/>
     <hyperlink ref="R117" r:id="rId11" display="Arrow"/>
-    <hyperlink ref="R122" r:id="rId12" display="Mouser"/>
+    <hyperlink ref="R122" r:id="rId12" display="Mouser,RAL Dig Lab, ADCMP605BCPZ-R7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="landscape"/>
@@ -27210,7 +27230,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="14" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="5"/>
@@ -27270,7 +27290,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44852</v>
+        <v>44944</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -27297,13 +27317,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:26">
       <c r="A5" s="8" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>7</v>
@@ -27345,7 +27365,7 @@
         <v>0.1</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>23</v>
@@ -27387,7 +27407,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>23</v>
@@ -27429,7 +27449,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>23</v>
@@ -27471,7 +27491,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>23</v>
@@ -27513,7 +27533,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>23</v>
@@ -27552,10 +27572,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>23</v>
@@ -27564,7 +27584,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>26</v>
@@ -27597,7 +27617,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>23</v>
@@ -27639,7 +27659,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>23</v>
@@ -27681,7 +27701,7 @@
         <v>43</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>23</v>
@@ -27721,16 +27741,16 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>26</v>
@@ -27761,16 +27781,16 @@
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>26</v>
@@ -27801,16 +27821,16 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>387</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>384</v>
-      </c>
       <c r="F17" s="12" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>26</v>
@@ -27841,7 +27861,7 @@
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>94</v>
@@ -27881,16 +27901,16 @@
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>26</v>
@@ -27921,16 +27941,16 @@
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>26</v>
@@ -27961,16 +27981,16 @@
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>26</v>
@@ -28001,16 +28021,16 @@
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>26</v>
@@ -28041,16 +28061,16 @@
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>26</v>
@@ -28081,16 +28101,16 @@
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>26</v>
@@ -28121,13 +28141,13 @@
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>117</v>
@@ -28161,16 +28181,16 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>26</v>
@@ -28201,16 +28221,16 @@
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>26</v>
@@ -28241,16 +28261,16 @@
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>26</v>
@@ -28281,16 +28301,16 @@
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="G29" s="18" t="s">
         <v>26</v>
@@ -28321,7 +28341,7 @@
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>125</v>
@@ -28363,7 +28383,7 @@
         <v>120</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>121</v>
@@ -28402,10 +28422,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>133</v>
@@ -28414,7 +28434,7 @@
         <v>134</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>26</v>
@@ -28445,16 +28465,16 @@
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>26</v>
@@ -28487,7 +28507,7 @@
         <v>100</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>163</v>
@@ -28529,7 +28549,7 @@
         <v>177</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>163</v>
@@ -28571,7 +28591,7 @@
         <v>3.01</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>163</v>
@@ -28580,7 +28600,7 @@
         <v>36</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>26</v>
@@ -28613,7 +28633,7 @@
         <v>204</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>163</v>
@@ -28655,7 +28675,7 @@
         <v>173</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>163</v>
@@ -28697,7 +28717,7 @@
         <v>198</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>163</v>
@@ -28739,7 +28759,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>163</v>
@@ -28781,7 +28801,7 @@
         <v>196</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>163</v>
@@ -28820,10 +28840,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>163</v>
@@ -28832,7 +28852,7 @@
         <v>36</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="G42" s="18" t="s">
         <v>26</v>
@@ -28862,10 +28882,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>163</v>
@@ -28874,7 +28894,7 @@
         <v>36</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="G43" s="18" t="s">
         <v>26</v>
@@ -28904,10 +28924,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>163</v>
@@ -28916,7 +28936,7 @@
         <v>36</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>26</v>
@@ -28949,7 +28969,7 @@
         <v>236</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>163</v>
@@ -28988,19 +29008,19 @@
         <v>8</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>163</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="G46" s="18" t="s">
         <v>26</v>
@@ -29031,16 +29051,16 @@
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="G47" s="18" t="s">
         <v>26</v>
@@ -29071,16 +29091,16 @@
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G48" s="18" t="s">
         <v>26</v>
@@ -29111,16 +29131,16 @@
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G49" s="18" t="s">
         <v>26</v>
@@ -29151,16 +29171,16 @@
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="G50" s="18" t="s">
         <v>26</v>
@@ -29191,16 +29211,16 @@
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>26</v>
@@ -29231,16 +29251,16 @@
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="G52" s="18" t="s">
         <v>26</v>
@@ -29271,16 +29291,16 @@
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="G53" s="18" t="s">
         <v>26</v>
@@ -29311,16 +29331,16 @@
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="12" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G54" s="18" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
received: 10 * AD5686RBCPZ-R7.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="491">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -1050,6 +1050,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF800080"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Winsource</t>
     </r>
     <r>
@@ -1570,11 +1577,11 @@
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="180" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -1694,14 +1701,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1718,14 +1732,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1739,30 +1746,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1770,14 +1754,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1791,16 +1775,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1823,6 +1807,29 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1932,13 +1939,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1950,37 +1963,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1992,73 +1987,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2070,31 +1999,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2107,6 +2018,102 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2516,11 +2523,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2540,26 +2553,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2575,17 +2568,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2607,145 +2614,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2760,7 +2767,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2785,7 +2792,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2811,7 +2818,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2983,58 +2990,58 @@
     <xf numFmtId="176" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3169,16 +3176,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3452,9 +3459,9 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D8" activePane="bottomLeft"/>
+      <pane ySplit="1170" topLeftCell="D72" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R8" sqref="R8"/>
+      <selection pane="bottomLeft" activeCell="T104" sqref="T104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3573,7 +3580,7 @@
       <c r="C5" s="35"/>
       <c r="D5" s="36">
         <f ca="1">TODAY()</f>
-        <v>44945</v>
+        <v>44958</v>
       </c>
       <c r="E5" s="75"/>
       <c r="F5" s="35"/>
@@ -6998,7 +7005,7 @@
       </c>
       <c r="P71" s="104"/>
       <c r="Q71" s="104">
-        <f>$N71+$P71</f>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="R71" s="120" t="s">
@@ -8820,16 +8827,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N106" s="110"/>
+      <c r="N106" s="110">
+        <v>10</v>
+      </c>
       <c r="O106" s="110">
         <v>631.68</v>
       </c>
       <c r="P106" s="110"/>
       <c r="Q106" s="110">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R106" s="123"/>
+        <v>10</v>
+      </c>
+      <c r="R106" s="123" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="107" ht="13" customHeight="1" spans="1:18">
       <c r="A107" s="48">
@@ -27511,7 +27522,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="7">
         <f ca="1">TODAY()</f>
-        <v>44945</v>
+        <v>44958</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>

</xml_diff>

<commit_message>
received: 16 * XC7K160T-2FFG676I, 16 * XC7K160T-2FFG676I.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12270" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="quabo" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="507">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -831,6 +831,9 @@
     <t>4/20/2022</t>
   </si>
   <si>
+    <t>16 * XC7K160T-2FFG676I</t>
+  </si>
+  <si>
     <t>LTC6090IS8E</t>
   </si>
   <si>
@@ -894,40 +897,43 @@
     <t>296-23564-1-ND</t>
   </si>
   <si>
+    <t>Winsource RAL Dig Lab</t>
+  </si>
+  <si>
+    <t>LP5951MF-3.0/NOPB</t>
+  </si>
+  <si>
+    <t>MF05A_N</t>
+  </si>
+  <si>
+    <t>LP5951MF-3.0/NOPBCT-ND</t>
+  </si>
+  <si>
+    <t>VM53S3</t>
+  </si>
+  <si>
+    <t>VM53S3-25.000-2.5/-30+85</t>
+  </si>
+  <si>
+    <t>Dove</t>
+  </si>
+  <si>
+    <t>Dan have some. we also received 7 from Linclon.</t>
+  </si>
+  <si>
+    <t>CDCM61004RHB</t>
+  </si>
+  <si>
+    <t>QFN32</t>
+  </si>
+  <si>
+    <t>296-24194-1-ND</t>
+  </si>
+  <si>
+    <t>9/22/2022</t>
+  </si>
+  <si>
     <t>Winsource</t>
-  </si>
-  <si>
-    <t>LP5951MF-3.0/NOPB</t>
-  </si>
-  <si>
-    <t>MF05A_N</t>
-  </si>
-  <si>
-    <t>LP5951MF-3.0/NOPBCT-ND</t>
-  </si>
-  <si>
-    <t>VM53S3</t>
-  </si>
-  <si>
-    <t>VM53S3-25.000-2.5/-30+85</t>
-  </si>
-  <si>
-    <t>Dove</t>
-  </si>
-  <si>
-    <t>Dan have some. we also received 7 from Linclon.</t>
-  </si>
-  <si>
-    <t>CDCM61004RHB</t>
-  </si>
-  <si>
-    <t>QFN32</t>
-  </si>
-  <si>
-    <t>296-24194-1-ND</t>
-  </si>
-  <si>
-    <t>9/22/2022</t>
   </si>
   <si>
     <t>AD5662BRJ-1REEL7</t>
@@ -1620,13 +1626,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -1745,8 +1751,119 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1761,49 +1878,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -1813,78 +1887,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1978,13 +1984,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1996,37 +2104,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2038,7 +2134,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2050,115 +2164,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2563,7 +2569,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2579,21 +2585,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2627,8 +2618,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2647,157 +2662,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="27" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2833,10 +2839,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2848,7 +2854,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2870,7 +2876,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2896,7 +2902,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2983,14 +2989,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3002,7 +3008,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3017,7 +3023,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3041,55 +3047,55 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3185,16 +3191,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3221,16 +3227,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3503,10 +3509,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" topLeftCell="E6" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
       <pane ySplit="1170" topLeftCell="D93" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
+      <selection pane="bottomLeft" activeCell="R100" sqref="R100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -8228,16 +8234,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N94" s="109"/>
+      <c r="N94" s="109">
+        <v>16</v>
+      </c>
       <c r="O94" s="109">
         <v>19174.4</v>
       </c>
       <c r="P94" s="109"/>
       <c r="Q94" s="109">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R94" s="122"/>
+        <v>16</v>
+      </c>
+      <c r="R94" s="122" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="95" ht="12.75" customHeight="1" spans="1:18">
       <c r="A95" s="58">
@@ -8248,19 +8258,19 @@
       </c>
       <c r="C95" s="59"/>
       <c r="D95" s="60" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E95" s="60" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F95" s="60" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G95" s="88" t="s">
         <v>26</v>
       </c>
       <c r="H95" s="89" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I95" s="106">
         <v>9.23</v>
@@ -8305,13 +8315,13 @@
       </c>
       <c r="C96" s="132"/>
       <c r="D96" s="132" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E96" s="132" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F96" s="132" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G96" s="97" t="s">
         <v>26</v>
@@ -8348,7 +8358,7 @@
         <v>51</v>
       </c>
       <c r="R96" s="127" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" ht="12.75" customHeight="1" spans="1:18">
@@ -8360,13 +8370,13 @@
       </c>
       <c r="C97" s="59"/>
       <c r="D97" s="60" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E97" s="60" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F97" s="60" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G97" s="88" t="s">
         <v>26</v>
@@ -8417,13 +8427,13 @@
       </c>
       <c r="C98" s="134"/>
       <c r="D98" s="134" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E98" s="134" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F98" s="134" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G98" s="149" t="s">
         <v>26</v>
@@ -8472,19 +8482,19 @@
       </c>
       <c r="C99" s="136"/>
       <c r="D99" s="137" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E99" s="137" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F99" s="137" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G99" s="93" t="s">
         <v>26</v>
       </c>
       <c r="H99" s="94" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="I99" s="110">
         <v>24.18</v>
@@ -8521,13 +8531,13 @@
       </c>
       <c r="C100" s="132"/>
       <c r="D100" s="132" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E100" s="132" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F100" s="132" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G100" s="97" t="s">
         <v>26</v>
@@ -8550,7 +8560,9 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N100" s="115"/>
+      <c r="N100" s="115">
+        <v>25</v>
+      </c>
       <c r="O100" s="115">
         <v>1584</v>
       </c>
@@ -8559,10 +8571,10 @@
       </c>
       <c r="Q100" s="115">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="R100" s="127" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="101" ht="14" customHeight="1" spans="1:18">
@@ -8574,13 +8586,13 @@
       </c>
       <c r="C101" s="59"/>
       <c r="D101" s="60" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E101" s="60" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F101" s="60" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G101" s="88" t="s">
         <v>26</v>
@@ -8631,16 +8643,16 @@
       </c>
       <c r="C102" s="54"/>
       <c r="D102" s="54" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E102" s="54" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F102" s="54" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G102" s="88" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H102" s="89" t="s">
         <v>39</v>
@@ -8672,7 +8684,7 @@
         <v>70</v>
       </c>
       <c r="R102" s="121" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="103" ht="12.75" customHeight="1" spans="1:18">
@@ -8684,19 +8696,19 @@
       </c>
       <c r="C103" s="67"/>
       <c r="D103" s="68" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E103" s="68" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F103" s="68" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G103" s="97" t="s">
         <v>26</v>
       </c>
       <c r="H103" s="98" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I103" s="114">
         <v>10.87</v>
@@ -8725,7 +8737,7 @@
         <v>10</v>
       </c>
       <c r="R103" s="127" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
     </row>
     <row r="104" ht="13" customHeight="1" spans="1:18">
@@ -8737,19 +8749,19 @@
       </c>
       <c r="C104" s="132"/>
       <c r="D104" s="132" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E104" s="132" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F104" s="132" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="G104" s="97" t="s">
         <v>26</v>
       </c>
       <c r="H104" s="98" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="I104" s="114">
         <v>8.55</v>
@@ -8780,7 +8792,7 @@
         <v>17</v>
       </c>
       <c r="R104" s="127" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="105" ht="13" customHeight="1" spans="1:18">
@@ -8792,19 +8804,19 @@
       </c>
       <c r="C105" s="67"/>
       <c r="D105" s="68" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E105" s="68" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F105" s="68" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G105" s="97" t="s">
         <v>26</v>
       </c>
       <c r="H105" s="98" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I105" s="114">
         <v>10.87</v>
@@ -8831,7 +8843,7 @@
         <v>0</v>
       </c>
       <c r="R105" s="127" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="106" ht="12" customHeight="1" spans="1:18">
@@ -8843,13 +8855,13 @@
       </c>
       <c r="C106" s="62"/>
       <c r="D106" s="62" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E106" s="62" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F106" s="62" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="G106" s="93" t="s">
         <v>26</v>
@@ -8896,19 +8908,19 @@
       </c>
       <c r="C107" s="56"/>
       <c r="D107" s="57" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E107" s="57" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F107" s="57" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G107" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H107" s="91" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="I107" s="108">
         <v>6.71</v>
@@ -8939,7 +8951,7 @@
         <v>13</v>
       </c>
       <c r="R107" s="122" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="108" ht="12.75" customHeight="1" spans="1:18">
@@ -8951,19 +8963,19 @@
       </c>
       <c r="C108" s="62"/>
       <c r="D108" s="62" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E108" s="62" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F108" s="62" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G108" s="93" t="s">
         <v>26</v>
       </c>
       <c r="H108" s="94" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="I108" s="110">
         <v>7.97</v>
@@ -8992,7 +9004,7 @@
         <v>8</v>
       </c>
       <c r="R108" s="123" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="109" ht="12.75" customHeight="1" spans="1:18">
@@ -9004,19 +9016,19 @@
       </c>
       <c r="C109" s="59"/>
       <c r="D109" s="60" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E109" s="60" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F109" s="60" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G109" s="88" t="s">
         <v>26</v>
       </c>
       <c r="H109" s="89" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="I109" s="106">
         <v>5.14</v>
@@ -9059,19 +9071,19 @@
       </c>
       <c r="C110" s="54"/>
       <c r="D110" s="54" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E110" s="54" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F110" s="54" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="G110" s="88" t="s">
         <v>26</v>
       </c>
       <c r="H110" s="89" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="I110" s="106">
         <v>51.06</v>
@@ -9114,13 +9126,13 @@
       </c>
       <c r="C111" s="59"/>
       <c r="D111" s="60" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E111" s="60" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F111" s="60" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G111" s="88" t="s">
         <v>26</v>
@@ -9171,13 +9183,13 @@
       </c>
       <c r="C112" s="54"/>
       <c r="D112" s="54" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E112" s="54" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="F112" s="54" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G112" s="88" t="s">
         <v>26</v>
@@ -9226,13 +9238,13 @@
       </c>
       <c r="C113" s="67"/>
       <c r="D113" s="68" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E113" s="68" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F113" s="68" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G113" s="97" t="s">
         <v>26</v>
@@ -9269,7 +9281,7 @@
         <v>26</v>
       </c>
       <c r="R113" s="127" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="114" ht="13" customHeight="1" spans="1:18">
@@ -9281,19 +9293,19 @@
       </c>
       <c r="C114" s="130"/>
       <c r="D114" s="130" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E114" s="130" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F114" s="130" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G114" s="90" t="s">
         <v>26</v>
       </c>
       <c r="H114" s="91" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="I114" s="108">
         <v>5.87</v>
@@ -9334,13 +9346,13 @@
       </c>
       <c r="C115" s="67"/>
       <c r="D115" s="68" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E115" s="68" t="s">
         <v>145</v>
       </c>
       <c r="F115" s="68" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G115" s="97" t="s">
         <v>26</v>
@@ -9377,7 +9389,7 @@
         <v>8</v>
       </c>
       <c r="R115" s="166" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="116" ht="12" customHeight="1" spans="1:18">
@@ -9389,10 +9401,10 @@
       </c>
       <c r="C116" s="54"/>
       <c r="D116" s="54" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E116" s="54" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F116" s="54" t="s">
         <v>77</v>
@@ -9436,13 +9448,13 @@
       </c>
       <c r="C117" s="67"/>
       <c r="D117" s="68" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E117" s="68" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="F117" s="68" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="G117" s="97" t="s">
         <v>26</v>
@@ -9477,7 +9489,7 @@
         <v>8</v>
       </c>
       <c r="R117" s="127" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="118" ht="13" customHeight="1" spans="1:18">
@@ -9489,19 +9501,19 @@
       </c>
       <c r="C118" s="62"/>
       <c r="D118" s="62" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E118" s="62" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F118" s="62" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="G118" s="93" t="s">
         <v>26</v>
       </c>
       <c r="H118" s="94" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="I118" s="110">
         <v>5.87</v>
@@ -9530,7 +9542,7 @@
         <v>42</v>
       </c>
       <c r="R118" s="123" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="119" ht="12.75" customHeight="1" spans="1:18">
@@ -9542,19 +9554,19 @@
       </c>
       <c r="C119" s="59"/>
       <c r="D119" s="60" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E119" s="60" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F119" s="60" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="G119" s="88" t="s">
         <v>26</v>
       </c>
       <c r="H119" s="89" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="I119" s="106">
         <v>7.34</v>
@@ -9599,19 +9611,19 @@
       </c>
       <c r="C120" s="54"/>
       <c r="D120" s="54" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E120" s="54" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="F120" s="54" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="G120" s="88" t="s">
         <v>26</v>
       </c>
       <c r="H120" s="89" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="I120" s="106">
         <v>4.94</v>
@@ -9656,19 +9668,19 @@
       </c>
       <c r="C121" s="59"/>
       <c r="D121" s="60" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E121" s="60" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F121" s="60" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="G121" s="88" t="s">
         <v>26</v>
       </c>
       <c r="H121" s="89" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="I121" s="106">
         <v>9.64</v>
@@ -9711,13 +9723,13 @@
       </c>
       <c r="C122" s="132"/>
       <c r="D122" s="132" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E122" s="132" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F122" s="132" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G122" s="97" t="s">
         <v>127</v>
@@ -9750,7 +9762,7 @@
         <v>10</v>
       </c>
       <c r="R122" s="127" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="123" ht="12.75" customHeight="1" spans="1:18">
@@ -9761,16 +9773,16 @@
         <v>39</v>
       </c>
       <c r="C123" s="64" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D123" s="65" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E123" s="65" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="F123" s="65" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G123" s="95" t="s">
         <v>127</v>
@@ -9813,19 +9825,19 @@
       </c>
       <c r="C124" s="139"/>
       <c r="D124" s="139" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E124" s="139" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="F124" s="139" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="G124" s="152" t="s">
         <v>26</v>
       </c>
       <c r="H124" s="94" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="I124" s="110">
         <v>5.83</v>
@@ -9856,7 +9868,7 @@
         <v>16</v>
       </c>
       <c r="R124" s="123" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="125" ht="28" customHeight="1" spans="1:18">
@@ -9869,7 +9881,7 @@
       <c r="G125" s="153"/>
       <c r="H125" s="154"/>
       <c r="I125" s="162" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="J125" s="163">
         <f>SUM(J6:J124)</f>
@@ -9911,7 +9923,7 @@
       <c r="A127" s="144"/>
       <c r="B127" s="145"/>
       <c r="C127" s="145" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D127" s="144"/>
       <c r="E127" s="145"/>
@@ -9939,7 +9951,7 @@
       <c r="A128" s="146"/>
       <c r="B128" s="146"/>
       <c r="C128" s="146" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D128" s="147"/>
       <c r="E128" s="146"/>
@@ -9967,13 +9979,13 @@
       <c r="A129" s="146"/>
       <c r="B129" s="146"/>
       <c r="C129" s="146" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D129" s="147"/>
       <c r="E129" s="146"/>
       <c r="F129" s="146"/>
       <c r="G129" s="158" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="H129" s="159"/>
       <c r="I129" s="104"/>
@@ -27441,7 +27453,7 @@
     <hyperlink ref="R49" r:id="rId3" display="RAL Dig Lab"/>
     <hyperlink ref="R51" r:id="rId4" display="Rochester, RAL Dig Lab. They are from digi-key"/>
     <hyperlink ref="R96" r:id="rId5" display="Winsource, RAL Dig Lab"/>
-    <hyperlink ref="R100" r:id="rId6" display="Winsource"/>
+    <hyperlink ref="R100" r:id="rId6" display="Winsource RAL Dig Lab"/>
     <hyperlink ref="R103" r:id="rId7" display="Winsource"/>
     <hyperlink ref="R104" r:id="rId8" display="Rochester, RAL Dig Lab"/>
     <hyperlink ref="R105" r:id="rId7" display="WinSource"/>
@@ -27507,7 +27519,7 @@
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="26" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="F2" s="27"/>
       <c r="G2" s="17"/>
@@ -27594,13 +27606,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:26">
       <c r="A5" s="20" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>7</v>
@@ -27642,7 +27654,7 @@
         <v>0.1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>23</v>
@@ -27684,7 +27696,7 @@
         <v>61</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>23</v>
@@ -27726,7 +27738,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>23</v>
@@ -27768,7 +27780,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>23</v>
@@ -27810,7 +27822,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>23</v>
@@ -27849,10 +27861,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>23</v>
@@ -27861,7 +27873,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>26</v>
@@ -27894,7 +27906,7 @@
         <v>75</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>23</v>
@@ -27936,7 +27948,7 @@
         <v>54</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>23</v>
@@ -27978,7 +27990,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>23</v>
@@ -28018,16 +28030,16 @@
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="G15" s="30" t="s">
         <v>26</v>
@@ -28058,16 +28070,16 @@
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="G16" s="30" t="s">
         <v>26</v>
@@ -28098,16 +28110,16 @@
       </c>
       <c r="B17" s="24"/>
       <c r="C17" s="24" t="s">
+        <v>393</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>394</v>
+      </c>
+      <c r="E17" s="24" t="s">
         <v>391</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>392</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>389</v>
-      </c>
       <c r="F17" s="24" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="G17" s="30" t="s">
         <v>26</v>
@@ -28138,7 +28150,7 @@
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="24" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>95</v>
@@ -28178,16 +28190,16 @@
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G19" s="30" t="s">
         <v>26</v>
@@ -28218,16 +28230,16 @@
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="24" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G20" s="30" t="s">
         <v>26</v>
@@ -28258,16 +28270,16 @@
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>26</v>
@@ -28298,16 +28310,16 @@
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="24" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>26</v>
@@ -28338,16 +28350,16 @@
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="24" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G23" s="30" t="s">
         <v>26</v>
@@ -28378,16 +28390,16 @@
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="G24" s="30" t="s">
         <v>26</v>
@@ -28418,13 +28430,13 @@
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="24" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>117</v>
@@ -28458,16 +28470,16 @@
       </c>
       <c r="B26" s="24"/>
       <c r="C26" s="24" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="G26" s="30" t="s">
         <v>26</v>
@@ -28498,16 +28510,16 @@
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="24" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="G27" s="30" t="s">
         <v>26</v>
@@ -28538,16 +28550,16 @@
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="G28" s="30" t="s">
         <v>26</v>
@@ -28578,16 +28590,16 @@
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="24" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="G29" s="30" t="s">
         <v>26</v>
@@ -28618,7 +28630,7 @@
       </c>
       <c r="B30" s="24"/>
       <c r="C30" s="24" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>125</v>
@@ -28660,7 +28672,7 @@
         <v>120</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>121</v>
@@ -28699,10 +28711,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>133</v>
@@ -28711,7 +28723,7 @@
         <v>134</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="G32" s="30" t="s">
         <v>26</v>
@@ -28742,16 +28754,16 @@
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="G33" s="30" t="s">
         <v>26</v>
@@ -28784,7 +28796,7 @@
         <v>100</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>163</v>
@@ -28826,7 +28838,7 @@
         <v>178</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>163</v>
@@ -28868,7 +28880,7 @@
         <v>3.01</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>163</v>
@@ -28877,7 +28889,7 @@
         <v>37</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="G36" s="30" t="s">
         <v>26</v>
@@ -28910,7 +28922,7 @@
         <v>207</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>163</v>
@@ -28952,7 +28964,7 @@
         <v>173</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>163</v>
@@ -28994,7 +29006,7 @@
         <v>201</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>163</v>
@@ -29036,7 +29048,7 @@
         <v>77</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>163</v>
@@ -29078,7 +29090,7 @@
         <v>199</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>163</v>
@@ -29117,10 +29129,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>163</v>
@@ -29129,7 +29141,7 @@
         <v>37</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="G42" s="30" t="s">
         <v>26</v>
@@ -29159,10 +29171,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>163</v>
@@ -29171,7 +29183,7 @@
         <v>37</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="G43" s="30" t="s">
         <v>26</v>
@@ -29201,10 +29213,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D44" s="24" t="s">
         <v>163</v>
@@ -29213,7 +29225,7 @@
         <v>37</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="G44" s="30" t="s">
         <v>26</v>
@@ -29246,7 +29258,7 @@
         <v>239</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D45" s="24" t="s">
         <v>163</v>
@@ -29285,19 +29297,19 @@
         <v>8</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="D46" s="24" t="s">
         <v>163</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="G46" s="30" t="s">
         <v>26</v>
@@ -29328,16 +29340,16 @@
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="G47" s="30" t="s">
         <v>26</v>
@@ -29368,16 +29380,16 @@
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="24" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="G48" s="30" t="s">
         <v>26</v>
@@ -29408,16 +29420,16 @@
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="24" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G49" s="30" t="s">
         <v>26</v>
@@ -29448,16 +29460,16 @@
       </c>
       <c r="B50" s="24"/>
       <c r="C50" s="24" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="G50" s="30" t="s">
         <v>26</v>
@@ -29488,16 +29500,16 @@
       </c>
       <c r="B51" s="24"/>
       <c r="C51" s="24" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="G51" s="30" t="s">
         <v>26</v>
@@ -29528,16 +29540,16 @@
       </c>
       <c r="B52" s="24"/>
       <c r="C52" s="24" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="G52" s="30" t="s">
         <v>26</v>
@@ -29568,16 +29580,16 @@
       </c>
       <c r="B53" s="24"/>
       <c r="C53" s="24" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>26</v>
@@ -29608,16 +29620,16 @@
       </c>
       <c r="B54" s="24"/>
       <c r="C54" s="24" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E54" s="24" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G54" s="30" t="s">
         <v>26</v>
@@ -29684,7 +29696,7 @@
   <sheetPr/>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -29697,7 +29709,7 @@
   <sheetData>
     <row r="1" ht="76.5" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -29724,16 +29736,16 @@
         <v>12</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>17</v>
@@ -29756,13 +29768,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="F2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="G2" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="L2">
         <v>25</v>
@@ -29775,7 +29787,7 @@
         <v>25</v>
       </c>
       <c r="R2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -29783,13 +29795,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>502</v>
+      </c>
+      <c r="F3" t="s">
+        <v>503</v>
+      </c>
+      <c r="G3" t="s">
         <v>500</v>
-      </c>
-      <c r="F3" t="s">
-        <v>501</v>
-      </c>
-      <c r="G3" t="s">
-        <v>498</v>
       </c>
       <c r="L3">
         <v>25</v>
@@ -29802,7 +29814,7 @@
         <v>25</v>
       </c>
       <c r="R3" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -29810,16 +29822,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="E4" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="F4" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="G4" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="L4">
         <v>25</v>
@@ -29832,7 +29844,7 @@
         <v>25</v>
       </c>
       <c r="R4" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
received: 8 * LTC3611IWP#PBF-ND
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="507">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -1627,12 +1627,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -1743,14 +1743,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1759,45 +1751,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1812,16 +1773,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1841,8 +1819,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1855,6 +1848,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1862,25 +1871,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1984,37 +1984,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2032,13 +2044,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2050,19 +2062,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2074,43 +2086,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2122,7 +2122,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2134,19 +2134,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2158,13 +2158,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2567,9 +2567,44 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2589,50 +2624,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2644,6 +2635,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2668,145 +2668,145 @@
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="27" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2839,10 +2839,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2876,7 +2876,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3050,52 +3050,52 @@
     <xf numFmtId="176" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3227,16 +3227,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3512,7 +3512,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
       <pane ySplit="1170" topLeftCell="D93" activePane="bottomLeft"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="R100" sqref="R100"/>
+      <selection pane="bottomLeft" activeCell="R99" sqref="R99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3631,7 +3631,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="47">
         <f ca="1">TODAY()</f>
-        <v>44964</v>
+        <v>44973</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="46"/>
@@ -8511,16 +8511,20 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N99" s="111"/>
+      <c r="N99" s="111">
+        <v>8</v>
+      </c>
       <c r="O99" s="111">
         <v>773.76</v>
       </c>
       <c r="P99" s="111"/>
       <c r="Q99" s="111">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R99" s="123"/>
+        <v>8</v>
+      </c>
+      <c r="R99" s="123" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="100" ht="12.75" customHeight="1" spans="1:18">
       <c r="A100" s="131">
@@ -27579,7 +27583,7 @@
       <c r="C4" s="17"/>
       <c r="D4" s="19">
         <f ca="1">TODAY()</f>
-        <v>44964</v>
+        <v>44973</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>

</xml_diff>

<commit_message>
added a new bom list for review.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12270"/>
+    <workbookView windowHeight="17730"/>
   </bookViews>
   <sheets>
     <sheet name="quabo" sheetId="1" r:id="rId1"/>
@@ -1627,12 +1627,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="[$-C09]dd\-mmm\-yy"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -1743,6 +1743,28 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1750,15 +1772,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1773,9 +1797,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1787,9 +1819,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1803,9 +1835,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1813,22 +1844,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1848,17 +1864,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1868,29 +1891,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1984,25 +1984,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2014,13 +2074,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2032,97 +2092,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2140,7 +2116,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2152,7 +2128,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2164,7 +2152,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2567,6 +2567,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2576,11 +2600,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2590,6 +2620,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2609,36 +2654,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2647,166 +2662,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="27" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2839,10 +2839,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2854,7 +2854,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2876,7 +2876,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2902,7 +2902,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3050,52 +3050,52 @@
     <xf numFmtId="176" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3227,16 +3227,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3509,10 +3509,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F6" workbookViewId="0">
-      <pane ySplit="1170" topLeftCell="D93" activePane="bottomLeft"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="R99" sqref="R99"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A6" workbookViewId="0">
+      <pane ySplit="1320" topLeftCell="D85" activePane="topLeft"/>
+      <selection activeCell="A34" sqref="$A34:$XFD52"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3631,7 +3631,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="47">
         <f ca="1">TODAY()</f>
-        <v>44973</v>
+        <v>44985</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="46"/>
@@ -27583,7 +27583,7 @@
       <c r="C4" s="17"/>
       <c r="D4" s="19">
         <f ca="1">TODAY()</f>
-        <v>44973</v>
+        <v>44985</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>

</xml_diff>

<commit_message>
received: 10 * LT1965IMS8E-1.8#PBF-ND 50 * blank shutter board PCB.
</commit_message>
<xml_diff>
--- a/202204_Mobo_Quabo_BOM.xlsx
+++ b/202204_Mobo_Quabo_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17730"/>
+    <workbookView windowWidth="28800" windowHeight="12270" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="quabo" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="508">
   <si>
     <t>Bill of Mat'ls</t>
   </si>
@@ -978,7 +978,7 @@
     <t>1/24/2023</t>
   </si>
   <si>
-    <t>9*LT1965IMS8E-1.8#PBF + 4*LT1965EMS8E-1.8#PBF</t>
+    <t>9*LT1965IMS8E-1.8#PBF + 14*LT1965EMS8E-1.8#PBF</t>
   </si>
   <si>
     <t>LT8609S</t>
@@ -1620,19 +1620,22 @@
   <si>
     <t>TMC2209-LA-T</t>
   </si>
+  <si>
+    <t>blank pcb board</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="177" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="179" formatCode="[$-C09]dd\-mmm\-yy"/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -1752,47 +1755,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1800,22 +1765,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1827,8 +1776,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1844,7 +1800,46 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1858,15 +1853,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1880,15 +1881,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1984,13 +1987,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2008,25 +2017,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2038,7 +2035,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2056,7 +2065,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2068,13 +2089,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2086,31 +2125,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2122,49 +2161,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2589,17 +2592,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2611,15 +2603,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2639,6 +2622,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2653,157 +2665,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="27" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="33" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2839,10 +2842,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2854,7 +2857,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2876,7 +2879,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2902,7 +2905,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2989,14 +2992,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3008,7 +3011,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3023,7 +3026,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3047,55 +3050,55 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3191,16 +3194,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3227,16 +3230,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3509,10 +3512,10 @@
   <sheetPr/>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A6" workbookViewId="0">
-      <pane ySplit="1320" topLeftCell="D85" activePane="topLeft"/>
-      <selection activeCell="A34" sqref="$A34:$XFD52"/>
-      <selection pane="bottomLeft"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" topLeftCell="F6" workbookViewId="0">
+      <pane ySplit="1320" topLeftCell="D88" activePane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="R108" sqref="R108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3631,7 +3634,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="47">
         <f ca="1">TODAY()</f>
-        <v>44985</v>
+        <v>45000</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="46"/>
@@ -8942,7 +8945,7 @@
         <v>0</v>
       </c>
       <c r="N107" s="109">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O107" s="109">
         <v>858.88</v>
@@ -8952,7 +8955,7 @@
       </c>
       <c r="Q107" s="109">
         <f t="shared" si="15"/>
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="R107" s="122" t="s">
         <v>306</v>
@@ -27583,7 +27586,7 @@
       <c r="C4" s="17"/>
       <c r="D4" s="19">
         <f ca="1">TODAY()</f>
-        <v>44985</v>
+        <v>45000</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
@@ -29698,13 +29701,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="4"/>
   <cols>
     <col min="4" max="4" width="21.2857142857143" customWidth="1"/>
     <col min="6" max="6" width="23.8571428571429" customWidth="1"/>
@@ -29851,6 +29854,26 @@
         <v>501</v>
       </c>
     </row>
+    <row r="5" spans="1:18">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>507</v>
+      </c>
+      <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="N5">
+        <v>50</v>
+      </c>
+      <c r="Q5">
+        <v>50</v>
+      </c>
+      <c r="R5" t="s">
+        <v>501</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>